<commit_message>
improve display of reference controls in applied controls
</commit_message>
<xml_diff>
--- a/tools/enisa/enisa-5g-scm-v1.3.xlsx
+++ b/tools/enisa/enisa-5g-scm-v1.3.xlsx
@@ -674,7 +674,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>M1</t>
+          <t>5G-M1</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -691,7 +691,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>M2</t>
+          <t>5G-M2</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -708,7 +708,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>M3</t>
+          <t>5G-M3</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -725,7 +725,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>M4</t>
+          <t>5G-M4</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -742,7 +742,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>M5</t>
+          <t>5G-M5</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -759,7 +759,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>M6</t>
+          <t>5G-M6</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -776,7 +776,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>M7</t>
+          <t>5G-M7</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -793,7 +793,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>M8</t>
+          <t>5G-M8</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -810,7 +810,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>M9</t>
+          <t>5G-M9</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -827,7 +827,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>M10</t>
+          <t>5G-M10</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -844,7 +844,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>M11</t>
+          <t>5G-M11</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -861,7 +861,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>M12</t>
+          <t>5G-M12</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -878,7 +878,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>M13</t>
+          <t>5G-M13</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -895,7 +895,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>M14</t>
+          <t>5G-M14</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -912,7 +912,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>M15</t>
+          <t>5G-M15</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -929,7 +929,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>M16</t>
+          <t>5G-M16</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -946,7 +946,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>M17</t>
+          <t>5G-M17</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -963,7 +963,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>M18</t>
+          <t>5G-M18</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -980,7 +980,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>M19</t>
+          <t>5G-M19</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -997,7 +997,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>M20</t>
+          <t>5G-M20</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -1014,7 +1014,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>M21</t>
+          <t>5G-M21</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -1031,7 +1031,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>M22</t>
+          <t>5G-M22</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -1048,7 +1048,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>M23</t>
+          <t>5G-M23</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -1065,7 +1065,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>M24</t>
+          <t>5G-M24</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -1082,7 +1082,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>M25</t>
+          <t>5G-M25</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -1099,7 +1099,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>M26</t>
+          <t>5G-M26</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -1116,7 +1116,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>M27</t>
+          <t>5G-M27</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1133,7 +1133,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>M28</t>
+          <t>5G-M28</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1150,7 +1150,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>M29</t>
+          <t>5G-M29</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -1167,7 +1167,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>M30</t>
+          <t>5G-M30</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -1184,7 +1184,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>M31</t>
+          <t>5G-M31</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -1201,7 +1201,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>M32</t>
+          <t>5G-M32</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -1218,7 +1218,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>M33</t>
+          <t>5G-M33</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -1235,7 +1235,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>M34</t>
+          <t>5G-M34</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -1252,7 +1252,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>M35</t>
+          <t>5G-M35</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -1269,7 +1269,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>M36</t>
+          <t>5G-M36</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -1286,7 +1286,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>M37</t>
+          <t>5G-M37</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -1303,7 +1303,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>M38</t>
+          <t>5G-M38</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -1320,7 +1320,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>M39</t>
+          <t>5G-M39</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -1337,7 +1337,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>M40</t>
+          <t>5G-M40</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -1354,7 +1354,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>M41</t>
+          <t>5G-M41</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -1371,7 +1371,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>M42</t>
+          <t>5G-M42</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -1388,7 +1388,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>M43</t>
+          <t>5G-M43</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -1405,7 +1405,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>M44</t>
+          <t>5G-M44</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -1422,7 +1422,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>M45</t>
+          <t>5G-M45</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -1439,7 +1439,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>M46</t>
+          <t>5G-M46</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -1456,7 +1456,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>M47</t>
+          <t>5G-M47</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -1473,7 +1473,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>M48</t>
+          <t>5G-M48</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -1490,7 +1490,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>M49</t>
+          <t>5G-M49</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -1507,7 +1507,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>M50</t>
+          <t>5G-M50</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -1524,7 +1524,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>M51</t>
+          <t>5G-M51</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -1541,7 +1541,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>M52</t>
+          <t>5G-M52</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -1558,7 +1558,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>M53</t>
+          <t>5G-M53</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -1575,7 +1575,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>M54</t>
+          <t>5G-M54</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -1592,7 +1592,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>M55</t>
+          <t>5G-M55</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -1609,7 +1609,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>M56</t>
+          <t>5G-M56</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -1626,7 +1626,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>M57</t>
+          <t>5G-M57</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -1643,7 +1643,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>M58</t>
+          <t>5G-M58</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -1660,7 +1660,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>M59</t>
+          <t>5G-M59</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -1677,7 +1677,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>M60</t>
+          <t>5G-M60</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -1694,7 +1694,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>M61</t>
+          <t>5G-M61</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -1711,7 +1711,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>M62</t>
+          <t>5G-M62</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -1728,7 +1728,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>M63</t>
+          <t>5G-M63</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -1745,7 +1745,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>M64</t>
+          <t>5G-M64</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -1762,7 +1762,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>M65</t>
+          <t>5G-M65</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -1779,7 +1779,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>M66</t>
+          <t>5G-M66</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -1796,7 +1796,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>M67</t>
+          <t>5G-M67</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
@@ -1813,7 +1813,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>M68</t>
+          <t>5G-M68</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
@@ -1830,7 +1830,7 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>M69</t>
+          <t>5G-M69</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
@@ -1847,7 +1847,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>M70</t>
+          <t>5G-M70</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
@@ -1864,7 +1864,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>M71</t>
+          <t>5G-M71</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -1881,7 +1881,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>M72</t>
+          <t>5G-M72</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
@@ -1898,7 +1898,7 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>M73</t>
+          <t>5G-M73</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
@@ -1915,7 +1915,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>M74</t>
+          <t>5G-M74</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -1932,7 +1932,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>M75</t>
+          <t>5G-M75</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -1949,7 +1949,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>M76</t>
+          <t>5G-M76</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -1966,7 +1966,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>M77</t>
+          <t>5G-M77</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -1983,7 +1983,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>M78</t>
+          <t>5G-M78</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -2000,7 +2000,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>M79</t>
+          <t>5G-M79</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -2017,7 +2017,7 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>M80</t>
+          <t>5G-M80</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
@@ -2034,7 +2034,7 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>M81</t>
+          <t>5G-M81</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
@@ -2051,7 +2051,7 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>M82</t>
+          <t>5G-M82</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
@@ -2068,7 +2068,7 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>M83</t>
+          <t>5G-M83</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
@@ -2085,7 +2085,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>M84</t>
+          <t>5G-M84</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -2102,7 +2102,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>M85</t>
+          <t>5G-M85</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -2119,7 +2119,7 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>M86</t>
+          <t>5G-M86</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
@@ -2136,7 +2136,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>M87</t>
+          <t>5G-M87</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -2153,7 +2153,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>M88</t>
+          <t>5G-M88</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
@@ -2170,7 +2170,7 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>M89</t>
+          <t>5G-M89</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
@@ -2187,7 +2187,7 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>M90</t>
+          <t>5G-M90</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
@@ -2204,7 +2204,7 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>M91</t>
+          <t>5G-M91</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
@@ -2221,7 +2221,7 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>M92</t>
+          <t>5G-M92</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
@@ -2238,7 +2238,7 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>M93</t>
+          <t>5G-M93</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
@@ -2255,7 +2255,7 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>M94</t>
+          <t>5G-M94</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
@@ -2272,7 +2272,7 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>M95</t>
+          <t>5G-M95</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
@@ -2289,7 +2289,7 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>M96</t>
+          <t>5G-M96</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
@@ -2306,7 +2306,7 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>M97</t>
+          <t>5G-M97</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
@@ -2323,7 +2323,7 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>M98</t>
+          <t>5G-M98</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
@@ -2340,7 +2340,7 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>M99</t>
+          <t>5G-M99</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
@@ -2357,7 +2357,7 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>M100</t>
+          <t>5G-M100</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
@@ -2374,7 +2374,7 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>M101</t>
+          <t>5G-M101</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
@@ -2391,7 +2391,7 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>M102</t>
+          <t>5G-M102</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
@@ -2408,7 +2408,7 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>M103</t>
+          <t>5G-M103</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
@@ -2425,7 +2425,7 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>M104</t>
+          <t>5G-M104</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
@@ -2442,7 +2442,7 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>M105</t>
+          <t>5G-M105</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
@@ -2459,7 +2459,7 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>M106</t>
+          <t>5G-M106</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
@@ -2476,7 +2476,7 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>M107</t>
+          <t>5G-M107</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
@@ -2493,7 +2493,7 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>M108</t>
+          <t>5G-M108</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
@@ -2510,7 +2510,7 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>M109</t>
+          <t>5G-M109</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
@@ -2527,7 +2527,7 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>M110</t>
+          <t>5G-M110</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
@@ -2544,7 +2544,7 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>M111</t>
+          <t>5G-M111</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
@@ -2561,7 +2561,7 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>M112</t>
+          <t>5G-M112</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
@@ -2578,7 +2578,7 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>M113</t>
+          <t>5G-M113</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
@@ -2595,7 +2595,7 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>M114</t>
+          <t>5G-M114</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
@@ -2612,7 +2612,7 @@
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>M115</t>
+          <t>5G-M115</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
@@ -2629,7 +2629,7 @@
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>M116</t>
+          <t>5G-M116</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
@@ -2646,7 +2646,7 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>M117</t>
+          <t>5G-M117</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
@@ -2663,7 +2663,7 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>M118</t>
+          <t>5G-M118</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
@@ -2680,7 +2680,7 @@
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>M119</t>
+          <t>5G-M119</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
@@ -2697,7 +2697,7 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>M120</t>
+          <t>5G-M120</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
@@ -2714,7 +2714,7 @@
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>M121</t>
+          <t>5G-M121</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
@@ -2731,7 +2731,7 @@
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>M122</t>
+          <t>5G-M122</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
@@ -2748,7 +2748,7 @@
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>M123</t>
+          <t>5G-M123</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
@@ -2765,7 +2765,7 @@
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>M124</t>
+          <t>5G-M124</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
@@ -2782,7 +2782,7 @@
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>M125</t>
+          <t>5G-M125</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
@@ -2799,7 +2799,7 @@
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>M126</t>
+          <t>5G-M126</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
@@ -2816,7 +2816,7 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>M127</t>
+          <t>5G-M127</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
@@ -2833,7 +2833,7 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>M128</t>
+          <t>5G-M128</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
@@ -2850,7 +2850,7 @@
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>M129</t>
+          <t>5G-M129</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
@@ -2867,7 +2867,7 @@
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>M130</t>
+          <t>5G-M130</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
@@ -2884,7 +2884,7 @@
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>M131</t>
+          <t>5G-M131</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
@@ -2901,7 +2901,7 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>M132</t>
+          <t>5G-M132</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
@@ -2918,7 +2918,7 @@
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>M133</t>
+          <t>5G-M133</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
@@ -2935,7 +2935,7 @@
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>M134</t>
+          <t>5G-M134</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
@@ -2952,7 +2952,7 @@
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>M135</t>
+          <t>5G-M135</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
@@ -2969,7 +2969,7 @@
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>M136</t>
+          <t>5G-M136</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
@@ -2986,7 +2986,7 @@
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>M137</t>
+          <t>5G-M137</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
@@ -3003,7 +3003,7 @@
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>M138</t>
+          <t>5G-M138</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
@@ -3020,7 +3020,7 @@
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>M139</t>
+          <t>5G-M139</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
@@ -3037,7 +3037,7 @@
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>M140</t>
+          <t>5G-M140</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
@@ -3054,7 +3054,7 @@
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>M141</t>
+          <t>5G-M141</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
@@ -3071,7 +3071,7 @@
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>M142</t>
+          <t>5G-M142</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
@@ -3088,7 +3088,7 @@
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>M143</t>
+          <t>5G-M143</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
@@ -3105,7 +3105,7 @@
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>M144</t>
+          <t>5G-M144</t>
         </is>
       </c>
       <c r="B145" t="inlineStr">
@@ -3236,7 +3236,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>1:M1,1:M2,1:M3,1:M4,1:M5,1:M6</t>
+          <t>1:5G-M1,1:5G-M2,1:5G-M3,1:5G-M4,1:5G-M5,1:5G-M6</t>
         </is>
       </c>
     </row>
@@ -3280,7 +3280,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>1:M1,1:M2,1:M3,1:M4,1:M5,1:M6</t>
+          <t>1:5G-M1,1:5G-M2,1:5G-M3,1:5G-M4,1:5G-M5,1:5G-M6</t>
         </is>
       </c>
     </row>
@@ -3346,7 +3346,7 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>1:M7,1:M8,1:M9,1:M10,1:M11,1:M12,1:M13</t>
+          <t>1:5G-M7,1:5G-M8,1:5G-M9,1:5G-M10,1:5G-M11,1:5G-M12,1:5G-M13</t>
         </is>
       </c>
     </row>
@@ -3390,7 +3390,7 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>1:M7,1:M8,1:M9,1:M10,1:M11,1:M12,1:M13</t>
+          <t>1:5G-M7,1:5G-M8,1:5G-M9,1:5G-M10,1:5G-M11,1:5G-M12,1:5G-M13</t>
         </is>
       </c>
     </row>
@@ -3434,7 +3434,7 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>1:M7,1:M8,1:M9,1:M10,1:M11,1:M12,1:M13</t>
+          <t>1:5G-M7,1:5G-M8,1:5G-M9,1:5G-M10,1:5G-M11,1:5G-M12,1:5G-M13</t>
         </is>
       </c>
     </row>
@@ -3478,7 +3478,7 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>1:M7,1:M8,1:M9,1:M10,1:M11,1:M12,1:M13</t>
+          <t>1:5G-M7,1:5G-M8,1:5G-M9,1:5G-M10,1:5G-M11,1:5G-M12,1:5G-M13</t>
         </is>
       </c>
     </row>
@@ -3523,7 +3523,7 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>1:M7,1:M8,1:M9,1:M10,1:M11,1:M12,1:M13</t>
+          <t>1:5G-M7,1:5G-M8,1:5G-M9,1:5G-M10,1:5G-M11,1:5G-M12,1:5G-M13</t>
         </is>
       </c>
     </row>
@@ -3590,7 +3590,7 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>1:M14,1:M15,1:M16,1:M17,1:M18</t>
+          <t>1:5G-M14,1:5G-M15,1:5G-M16,1:5G-M17,1:5G-M18</t>
         </is>
       </c>
     </row>
@@ -3656,7 +3656,7 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>1:M19,1:M20,1:M21,1:M22,1:M23,1:M24,1:M25,1:M26</t>
+          <t>1:5G-M19,1:5G-M20,1:5G-M21,1:5G-M22,1:5G-M23,1:5G-M24,1:5G-M25,1:5G-M26</t>
         </is>
       </c>
     </row>
@@ -3700,7 +3700,7 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>1:M19,1:M20,1:M21,1:M22,1:M23,1:M24,1:M25,1:M26</t>
+          <t>1:5G-M19,1:5G-M20,1:5G-M21,1:5G-M22,1:5G-M23,1:5G-M24,1:5G-M25,1:5G-M26</t>
         </is>
       </c>
     </row>
@@ -3744,7 +3744,7 @@
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>1:M19,1:M20,1:M21,1:M22,1:M23,1:M24,1:M25,1:M26</t>
+          <t>1:5G-M19,1:5G-M20,1:5G-M21,1:5G-M22,1:5G-M23,1:5G-M24,1:5G-M25,1:5G-M26</t>
         </is>
       </c>
     </row>
@@ -3788,7 +3788,7 @@
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>1:M19,1:M20,1:M21,1:M22,1:M23,1:M24,1:M25,1:M26</t>
+          <t>1:5G-M19,1:5G-M20,1:5G-M21,1:5G-M22,1:5G-M23,1:5G-M24,1:5G-M25,1:5G-M26</t>
         </is>
       </c>
     </row>
@@ -3832,7 +3832,7 @@
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>1:M19,1:M20,1:M21,1:M22,1:M23,1:M24,1:M25,1:M26</t>
+          <t>1:5G-M19,1:5G-M20,1:5G-M21,1:5G-M22,1:5G-M23,1:5G-M24,1:5G-M25,1:5G-M26</t>
         </is>
       </c>
     </row>
@@ -3876,7 +3876,7 @@
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>1:M19,1:M20,1:M21,1:M22,1:M23,1:M24,1:M25,1:M26</t>
+          <t>1:5G-M19,1:5G-M20,1:5G-M21,1:5G-M22,1:5G-M23,1:5G-M24,1:5G-M25,1:5G-M26</t>
         </is>
       </c>
     </row>
@@ -3920,7 +3920,7 @@
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>1:M19,1:M20,1:M21,1:M22,1:M23,1:M24,1:M25,1:M26</t>
+          <t>1:5G-M19,1:5G-M20,1:5G-M21,1:5G-M22,1:5G-M23,1:5G-M24,1:5G-M25,1:5G-M26</t>
         </is>
       </c>
     </row>
@@ -3964,7 +3964,7 @@
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>1:M19,1:M20,1:M21,1:M22,1:M23,1:M24,1:M25,1:M26</t>
+          <t>1:5G-M19,1:5G-M20,1:5G-M21,1:5G-M22,1:5G-M23,1:5G-M24,1:5G-M25,1:5G-M26</t>
         </is>
       </c>
     </row>
@@ -4009,7 +4009,7 @@
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>1:M19,1:M20,1:M21,1:M22,1:M23,1:M24,1:M25,1:M26</t>
+          <t>1:5G-M19,1:5G-M20,1:5G-M21,1:5G-M22,1:5G-M23,1:5G-M24,1:5G-M25,1:5G-M26</t>
         </is>
       </c>
     </row>
@@ -4053,7 +4053,7 @@
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>1:M19,1:M20,1:M21,1:M22,1:M23,1:M24,1:M25,1:M26</t>
+          <t>1:5G-M19,1:5G-M20,1:5G-M21,1:5G-M22,1:5G-M23,1:5G-M24,1:5G-M25,1:5G-M26</t>
         </is>
       </c>
     </row>
@@ -4097,7 +4097,7 @@
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>1:M19,1:M20,1:M21,1:M22,1:M23,1:M24,1:M25,1:M26</t>
+          <t>1:5G-M19,1:5G-M20,1:5G-M21,1:5G-M22,1:5G-M23,1:5G-M24,1:5G-M25,1:5G-M26</t>
         </is>
       </c>
     </row>
@@ -4142,7 +4142,7 @@
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>1:M19,1:M20,1:M21,1:M22,1:M23,1:M24,1:M25,1:M26</t>
+          <t>1:5G-M19,1:5G-M20,1:5G-M21,1:5G-M22,1:5G-M23,1:5G-M24,1:5G-M25,1:5G-M26</t>
         </is>
       </c>
     </row>
@@ -4186,7 +4186,7 @@
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>1:M19,1:M20,1:M21,1:M22,1:M23,1:M24,1:M25,1:M26</t>
+          <t>1:5G-M19,1:5G-M20,1:5G-M21,1:5G-M22,1:5G-M23,1:5G-M24,1:5G-M25,1:5G-M26</t>
         </is>
       </c>
     </row>
@@ -4230,7 +4230,7 @@
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>1:M19,1:M20,1:M21,1:M22,1:M23,1:M24,1:M25,1:M26</t>
+          <t>1:5G-M19,1:5G-M20,1:5G-M21,1:5G-M22,1:5G-M23,1:5G-M24,1:5G-M25,1:5G-M26</t>
         </is>
       </c>
     </row>
@@ -4274,7 +4274,7 @@
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>1:M19,1:M20,1:M21,1:M22,1:M23,1:M24,1:M25,1:M26</t>
+          <t>1:5G-M19,1:5G-M20,1:5G-M21,1:5G-M22,1:5G-M23,1:5G-M24,1:5G-M25,1:5G-M26</t>
         </is>
       </c>
     </row>
@@ -4318,7 +4318,7 @@
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>1:M19,1:M20,1:M21,1:M22,1:M23,1:M24,1:M25,1:M26</t>
+          <t>1:5G-M19,1:5G-M20,1:5G-M21,1:5G-M22,1:5G-M23,1:5G-M24,1:5G-M25,1:5G-M26</t>
         </is>
       </c>
     </row>
@@ -4362,7 +4362,7 @@
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>1:M19,1:M20,1:M21,1:M22,1:M23,1:M24,1:M25,1:M26</t>
+          <t>1:5G-M19,1:5G-M20,1:5G-M21,1:5G-M22,1:5G-M23,1:5G-M24,1:5G-M25,1:5G-M26</t>
         </is>
       </c>
     </row>
@@ -4406,7 +4406,7 @@
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>1:M19,1:M20,1:M21,1:M22,1:M23,1:M24,1:M25,1:M26</t>
+          <t>1:5G-M19,1:5G-M20,1:5G-M21,1:5G-M22,1:5G-M23,1:5G-M24,1:5G-M25,1:5G-M26</t>
         </is>
       </c>
     </row>
@@ -4451,7 +4451,7 @@
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>1:M19,1:M20,1:M21,1:M22,1:M23,1:M24,1:M25,1:M26</t>
+          <t>1:5G-M19,1:5G-M20,1:5G-M21,1:5G-M22,1:5G-M23,1:5G-M24,1:5G-M25,1:5G-M26</t>
         </is>
       </c>
     </row>
@@ -4495,7 +4495,7 @@
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>1:M19,1:M20,1:M21,1:M22,1:M23,1:M24,1:M25,1:M26</t>
+          <t>1:5G-M19,1:5G-M20,1:5G-M21,1:5G-M22,1:5G-M23,1:5G-M24,1:5G-M25,1:5G-M26</t>
         </is>
       </c>
     </row>
@@ -4539,7 +4539,7 @@
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>1:M19,1:M20,1:M21,1:M22,1:M23,1:M24,1:M25,1:M26</t>
+          <t>1:5G-M19,1:5G-M20,1:5G-M21,1:5G-M22,1:5G-M23,1:5G-M24,1:5G-M25,1:5G-M26</t>
         </is>
       </c>
     </row>
@@ -4583,7 +4583,7 @@
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>1:M19,1:M20,1:M21,1:M22,1:M23,1:M24,1:M25,1:M26</t>
+          <t>1:5G-M19,1:5G-M20,1:5G-M21,1:5G-M22,1:5G-M23,1:5G-M24,1:5G-M25,1:5G-M26</t>
         </is>
       </c>
     </row>
@@ -4627,7 +4627,7 @@
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>1:M19,1:M20,1:M21,1:M22,1:M23,1:M24,1:M25,1:M26</t>
+          <t>1:5G-M19,1:5G-M20,1:5G-M21,1:5G-M22,1:5G-M23,1:5G-M24,1:5G-M25,1:5G-M26</t>
         </is>
       </c>
     </row>
@@ -4671,7 +4671,7 @@
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>1:M19,1:M20,1:M21,1:M22,1:M23,1:M24,1:M25,1:M26</t>
+          <t>1:5G-M19,1:5G-M20,1:5G-M21,1:5G-M22,1:5G-M23,1:5G-M24,1:5G-M25,1:5G-M26</t>
         </is>
       </c>
     </row>
@@ -4715,7 +4715,7 @@
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>1:M19,1:M20,1:M21,1:M22,1:M23,1:M24,1:M25,1:M26</t>
+          <t>1:5G-M19,1:5G-M20,1:5G-M21,1:5G-M22,1:5G-M23,1:5G-M24,1:5G-M25,1:5G-M26</t>
         </is>
       </c>
     </row>
@@ -4759,7 +4759,7 @@
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>1:M19,1:M20,1:M21,1:M22,1:M23,1:M24,1:M25,1:M26</t>
+          <t>1:5G-M19,1:5G-M20,1:5G-M21,1:5G-M22,1:5G-M23,1:5G-M24,1:5G-M25,1:5G-M26</t>
         </is>
       </c>
     </row>
@@ -4803,7 +4803,7 @@
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>1:M19,1:M20,1:M21,1:M22,1:M23,1:M24,1:M25,1:M26</t>
+          <t>1:5G-M19,1:5G-M20,1:5G-M21,1:5G-M22,1:5G-M23,1:5G-M24,1:5G-M25,1:5G-M26</t>
         </is>
       </c>
     </row>
@@ -4847,7 +4847,7 @@
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>1:M19,1:M20,1:M21,1:M22,1:M23,1:M24,1:M25,1:M26</t>
+          <t>1:5G-M19,1:5G-M20,1:5G-M21,1:5G-M22,1:5G-M23,1:5G-M24,1:5G-M25,1:5G-M26</t>
         </is>
       </c>
     </row>
@@ -4891,7 +4891,7 @@
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>1:M19,1:M20,1:M21,1:M22,1:M23,1:M24,1:M25,1:M26</t>
+          <t>1:5G-M19,1:5G-M20,1:5G-M21,1:5G-M22,1:5G-M23,1:5G-M24,1:5G-M25,1:5G-M26</t>
         </is>
       </c>
     </row>
@@ -4935,7 +4935,7 @@
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>1:M19,1:M20,1:M21,1:M22,1:M23,1:M24,1:M25,1:M26</t>
+          <t>1:5G-M19,1:5G-M20,1:5G-M21,1:5G-M22,1:5G-M23,1:5G-M24,1:5G-M25,1:5G-M26</t>
         </is>
       </c>
     </row>
@@ -4979,7 +4979,7 @@
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>1:M19,1:M20,1:M21,1:M22,1:M23,1:M24,1:M25,1:M26</t>
+          <t>1:5G-M19,1:5G-M20,1:5G-M21,1:5G-M22,1:5G-M23,1:5G-M24,1:5G-M25,1:5G-M26</t>
         </is>
       </c>
     </row>
@@ -5023,7 +5023,7 @@
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>1:M19,1:M20,1:M21,1:M22,1:M23,1:M24,1:M25,1:M26</t>
+          <t>1:5G-M19,1:5G-M20,1:5G-M21,1:5G-M22,1:5G-M23,1:5G-M24,1:5G-M25,1:5G-M26</t>
         </is>
       </c>
     </row>
@@ -5067,7 +5067,7 @@
       </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t>1:M19,1:M20,1:M21,1:M22,1:M23,1:M24,1:M25,1:M26</t>
+          <t>1:5G-M19,1:5G-M20,1:5G-M21,1:5G-M22,1:5G-M23,1:5G-M24,1:5G-M25,1:5G-M26</t>
         </is>
       </c>
     </row>
@@ -5111,7 +5111,7 @@
       </c>
       <c r="F89" t="inlineStr">
         <is>
-          <t>1:M19,1:M20,1:M21,1:M22,1:M23,1:M24,1:M25,1:M26</t>
+          <t>1:5G-M19,1:5G-M20,1:5G-M21,1:5G-M22,1:5G-M23,1:5G-M24,1:5G-M25,1:5G-M26</t>
         </is>
       </c>
     </row>
@@ -5155,7 +5155,7 @@
       </c>
       <c r="F91" t="inlineStr">
         <is>
-          <t>1:M19,1:M20,1:M21,1:M22,1:M23,1:M24,1:M25,1:M26</t>
+          <t>1:5G-M19,1:5G-M20,1:5G-M21,1:5G-M22,1:5G-M23,1:5G-M24,1:5G-M25,1:5G-M26</t>
         </is>
       </c>
     </row>
@@ -5199,7 +5199,7 @@
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>1:M19,1:M20,1:M21,1:M22,1:M23,1:M24,1:M25,1:M26</t>
+          <t>1:5G-M19,1:5G-M20,1:5G-M21,1:5G-M22,1:5G-M23,1:5G-M24,1:5G-M25,1:5G-M26</t>
         </is>
       </c>
     </row>
@@ -5243,7 +5243,7 @@
       </c>
       <c r="F95" t="inlineStr">
         <is>
-          <t>1:M19,1:M20,1:M21,1:M22,1:M23,1:M24,1:M25,1:M26</t>
+          <t>1:5G-M19,1:5G-M20,1:5G-M21,1:5G-M22,1:5G-M23,1:5G-M24,1:5G-M25,1:5G-M26</t>
         </is>
       </c>
     </row>
@@ -5289,7 +5289,7 @@
       </c>
       <c r="F97" t="inlineStr">
         <is>
-          <t>1:M19,1:M20,1:M21,1:M22,1:M23,1:M24,1:M25,1:M26</t>
+          <t>1:5G-M19,1:5G-M20,1:5G-M21,1:5G-M22,1:5G-M23,1:5G-M24,1:5G-M25,1:5G-M26</t>
         </is>
       </c>
     </row>
@@ -5335,7 +5335,7 @@
       </c>
       <c r="F99" t="inlineStr">
         <is>
-          <t>1:M19,1:M20,1:M21,1:M22,1:M23,1:M24,1:M25,1:M26</t>
+          <t>1:5G-M19,1:5G-M20,1:5G-M21,1:5G-M22,1:5G-M23,1:5G-M24,1:5G-M25,1:5G-M26</t>
         </is>
       </c>
     </row>
@@ -5380,7 +5380,7 @@
       </c>
       <c r="F101" t="inlineStr">
         <is>
-          <t>1:M19,1:M20,1:M21,1:M22,1:M23,1:M24,1:M25,1:M26</t>
+          <t>1:5G-M19,1:5G-M20,1:5G-M21,1:5G-M22,1:5G-M23,1:5G-M24,1:5G-M25,1:5G-M26</t>
         </is>
       </c>
     </row>
@@ -5432,7 +5432,7 @@
       </c>
       <c r="F103" t="inlineStr">
         <is>
-          <t>1:M19,1:M20,1:M21,1:M22,1:M23,1:M24,1:M25,1:M26</t>
+          <t>1:5G-M19,1:5G-M20,1:5G-M21,1:5G-M22,1:5G-M23,1:5G-M24,1:5G-M25,1:5G-M26</t>
         </is>
       </c>
     </row>
@@ -5476,7 +5476,7 @@
       </c>
       <c r="F105" t="inlineStr">
         <is>
-          <t>1:M19,1:M20,1:M21,1:M22,1:M23,1:M24,1:M25,1:M26</t>
+          <t>1:5G-M19,1:5G-M20,1:5G-M21,1:5G-M22,1:5G-M23,1:5G-M24,1:5G-M25,1:5G-M26</t>
         </is>
       </c>
     </row>
@@ -5520,7 +5520,7 @@
       </c>
       <c r="F107" t="inlineStr">
         <is>
-          <t>1:M19,1:M20,1:M21,1:M22,1:M23,1:M24,1:M25,1:M26</t>
+          <t>1:5G-M19,1:5G-M20,1:5G-M21,1:5G-M22,1:5G-M23,1:5G-M24,1:5G-M25,1:5G-M26</t>
         </is>
       </c>
     </row>
@@ -5564,7 +5564,7 @@
       </c>
       <c r="F109" t="inlineStr">
         <is>
-          <t>1:M19,1:M20,1:M21,1:M22,1:M23,1:M24,1:M25,1:M26</t>
+          <t>1:5G-M19,1:5G-M20,1:5G-M21,1:5G-M22,1:5G-M23,1:5G-M24,1:5G-M25,1:5G-M26</t>
         </is>
       </c>
     </row>
@@ -5608,7 +5608,7 @@
       </c>
       <c r="F111" t="inlineStr">
         <is>
-          <t>1:M19,1:M20,1:M21,1:M22,1:M23,1:M24,1:M25,1:M26</t>
+          <t>1:5G-M19,1:5G-M20,1:5G-M21,1:5G-M22,1:5G-M23,1:5G-M24,1:5G-M25,1:5G-M26</t>
         </is>
       </c>
     </row>
@@ -5652,7 +5652,7 @@
       </c>
       <c r="F113" t="inlineStr">
         <is>
-          <t>1:M19,1:M20,1:M21,1:M22,1:M23,1:M24,1:M25,1:M26</t>
+          <t>1:5G-M19,1:5G-M20,1:5G-M21,1:5G-M22,1:5G-M23,1:5G-M24,1:5G-M25,1:5G-M26</t>
         </is>
       </c>
     </row>
@@ -5696,7 +5696,7 @@
       </c>
       <c r="F115" t="inlineStr">
         <is>
-          <t>1:M19,1:M20,1:M21,1:M22,1:M23,1:M24,1:M25,1:M26</t>
+          <t>1:5G-M19,1:5G-M20,1:5G-M21,1:5G-M22,1:5G-M23,1:5G-M24,1:5G-M25,1:5G-M26</t>
         </is>
       </c>
     </row>
@@ -5784,7 +5784,7 @@
       </c>
       <c r="F119" t="inlineStr">
         <is>
-          <t>1:M27,1:M28,1:M29,1:M30</t>
+          <t>1:5G-M27,1:5G-M28,1:5G-M29,1:5G-M30</t>
         </is>
       </c>
     </row>
@@ -5850,7 +5850,7 @@
       </c>
       <c r="F122" t="inlineStr">
         <is>
-          <t>1:M31,1:M32,1:M33,1:M34,1:M35</t>
+          <t>1:5G-M31,1:5G-M32,1:5G-M33,1:5G-M34,1:5G-M35</t>
         </is>
       </c>
     </row>
@@ -5938,7 +5938,7 @@
       </c>
       <c r="F126" t="inlineStr">
         <is>
-          <t>1:M45,1:M46,1:M47,1:M48,1:M49,1:M50</t>
+          <t>1:5G-M45,1:5G-M46,1:5G-M47,1:5G-M48,1:5G-M49,1:5G-M50</t>
         </is>
       </c>
     </row>
@@ -5982,7 +5982,7 @@
       </c>
       <c r="F128" t="inlineStr">
         <is>
-          <t>1:M45,1:M46,1:M47,1:M48,1:M49,1:M50</t>
+          <t>1:5G-M45,1:5G-M46,1:5G-M47,1:5G-M48,1:5G-M49,1:5G-M50</t>
         </is>
       </c>
     </row>
@@ -6026,7 +6026,7 @@
       </c>
       <c r="F130" t="inlineStr">
         <is>
-          <t>1:M45,1:M46,1:M47,1:M48,1:M49,1:M50</t>
+          <t>1:5G-M45,1:5G-M46,1:5G-M47,1:5G-M48,1:5G-M49,1:5G-M50</t>
         </is>
       </c>
     </row>
@@ -6070,7 +6070,7 @@
       </c>
       <c r="F132" t="inlineStr">
         <is>
-          <t>1:M45,1:M46,1:M47,1:M48,1:M49,1:M50</t>
+          <t>1:5G-M45,1:5G-M46,1:5G-M47,1:5G-M48,1:5G-M49,1:5G-M50</t>
         </is>
       </c>
     </row>
@@ -6114,7 +6114,7 @@
       </c>
       <c r="F134" t="inlineStr">
         <is>
-          <t>1:M45,1:M46,1:M47,1:M48,1:M49,1:M50</t>
+          <t>1:5G-M45,1:5G-M46,1:5G-M47,1:5G-M48,1:5G-M49,1:5G-M50</t>
         </is>
       </c>
     </row>
@@ -6158,7 +6158,7 @@
       </c>
       <c r="F136" t="inlineStr">
         <is>
-          <t>1:M45,1:M46,1:M47,1:M48,1:M49,1:M50</t>
+          <t>1:5G-M45,1:5G-M46,1:5G-M47,1:5G-M48,1:5G-M49,1:5G-M50</t>
         </is>
       </c>
     </row>
@@ -6202,7 +6202,7 @@
       </c>
       <c r="F138" t="inlineStr">
         <is>
-          <t>1:M45,1:M46,1:M47,1:M48,1:M49,1:M50</t>
+          <t>1:5G-M45,1:5G-M46,1:5G-M47,1:5G-M48,1:5G-M49,1:5G-M50</t>
         </is>
       </c>
     </row>
@@ -6246,7 +6246,7 @@
       </c>
       <c r="F140" t="inlineStr">
         <is>
-          <t>1:M45,1:M46,1:M47,1:M48,1:M49,1:M50</t>
+          <t>1:5G-M45,1:5G-M46,1:5G-M47,1:5G-M48,1:5G-M49,1:5G-M50</t>
         </is>
       </c>
     </row>
@@ -6290,7 +6290,7 @@
       </c>
       <c r="F142" t="inlineStr">
         <is>
-          <t>1:M45,1:M46,1:M47,1:M48,1:M49,1:M50</t>
+          <t>1:5G-M45,1:5G-M46,1:5G-M47,1:5G-M48,1:5G-M49,1:5G-M50</t>
         </is>
       </c>
     </row>
@@ -6359,7 +6359,7 @@
       </c>
       <c r="F145" t="inlineStr">
         <is>
-          <t>1:M51,1:M52,1:M53,1:M54,1:M55</t>
+          <t>1:5G-M51,1:5G-M52,1:5G-M53,1:5G-M54,1:5G-M55</t>
         </is>
       </c>
     </row>
@@ -6425,7 +6425,7 @@
       </c>
       <c r="F148" t="inlineStr">
         <is>
-          <t>1:M56,1:M57,1:M58,1:M59,1:M60,1:M61,1:M62,1:M63</t>
+          <t>1:5G-M56,1:5G-M57,1:5G-M58,1:5G-M59,1:5G-M60,1:5G-M61,1:5G-M62,1:5G-M63</t>
         </is>
       </c>
     </row>
@@ -6469,7 +6469,7 @@
       </c>
       <c r="F150" t="inlineStr">
         <is>
-          <t>1:M56,1:M57,1:M58,1:M59,1:M60,1:M61,1:M62,1:M63</t>
+          <t>1:5G-M56,1:5G-M57,1:5G-M58,1:5G-M59,1:5G-M60,1:5G-M61,1:5G-M62,1:5G-M63</t>
         </is>
       </c>
     </row>
@@ -6513,7 +6513,7 @@
       </c>
       <c r="F152" t="inlineStr">
         <is>
-          <t>1:M56,1:M57,1:M58,1:M59,1:M60,1:M61,1:M62,1:M63</t>
+          <t>1:5G-M56,1:5G-M57,1:5G-M58,1:5G-M59,1:5G-M60,1:5G-M61,1:5G-M62,1:5G-M63</t>
         </is>
       </c>
     </row>
@@ -6558,7 +6558,7 @@
       </c>
       <c r="F154" t="inlineStr">
         <is>
-          <t>1:M56,1:M57,1:M58,1:M59,1:M60,1:M61,1:M62,1:M63</t>
+          <t>1:5G-M56,1:5G-M57,1:5G-M58,1:5G-M59,1:5G-M60,1:5G-M61,1:5G-M62,1:5G-M63</t>
         </is>
       </c>
     </row>
@@ -6602,7 +6602,7 @@
       </c>
       <c r="F156" t="inlineStr">
         <is>
-          <t>1:M56,1:M57,1:M58,1:M59,1:M60,1:M61,1:M62,1:M63</t>
+          <t>1:5G-M56,1:5G-M57,1:5G-M58,1:5G-M59,1:5G-M60,1:5G-M61,1:5G-M62,1:5G-M63</t>
         </is>
       </c>
     </row>
@@ -6646,7 +6646,7 @@
       </c>
       <c r="F158" t="inlineStr">
         <is>
-          <t>1:M56,1:M57,1:M58,1:M59,1:M60,1:M61,1:M62,1:M63</t>
+          <t>1:5G-M56,1:5G-M57,1:5G-M58,1:5G-M59,1:5G-M60,1:5G-M61,1:5G-M62,1:5G-M63</t>
         </is>
       </c>
     </row>
@@ -6690,7 +6690,7 @@
       </c>
       <c r="F160" t="inlineStr">
         <is>
-          <t>1:M56,1:M57,1:M58,1:M59,1:M60,1:M61,1:M62,1:M63</t>
+          <t>1:5G-M56,1:5G-M57,1:5G-M58,1:5G-M59,1:5G-M60,1:5G-M61,1:5G-M62,1:5G-M63</t>
         </is>
       </c>
     </row>
@@ -6734,7 +6734,7 @@
       </c>
       <c r="F162" t="inlineStr">
         <is>
-          <t>1:M56,1:M57,1:M58,1:M59,1:M60,1:M61,1:M62,1:M63</t>
+          <t>1:5G-M56,1:5G-M57,1:5G-M58,1:5G-M59,1:5G-M60,1:5G-M61,1:5G-M62,1:5G-M63</t>
         </is>
       </c>
     </row>
@@ -6779,7 +6779,7 @@
       </c>
       <c r="F164" t="inlineStr">
         <is>
-          <t>1:M56,1:M57,1:M58,1:M59,1:M60,1:M61,1:M62,1:M63</t>
+          <t>1:5G-M56,1:5G-M57,1:5G-M58,1:5G-M59,1:5G-M60,1:5G-M61,1:5G-M62,1:5G-M63</t>
         </is>
       </c>
     </row>
@@ -6823,7 +6823,7 @@
       </c>
       <c r="F166" t="inlineStr">
         <is>
-          <t>1:M56,1:M57,1:M58,1:M59,1:M60,1:M61,1:M62,1:M63</t>
+          <t>1:5G-M56,1:5G-M57,1:5G-M58,1:5G-M59,1:5G-M60,1:5G-M61,1:5G-M62,1:5G-M63</t>
         </is>
       </c>
     </row>
@@ -6867,7 +6867,7 @@
       </c>
       <c r="F168" t="inlineStr">
         <is>
-          <t>1:M56,1:M57,1:M58,1:M59,1:M60,1:M61,1:M62,1:M63</t>
+          <t>1:5G-M56,1:5G-M57,1:5G-M58,1:5G-M59,1:5G-M60,1:5G-M61,1:5G-M62,1:5G-M63</t>
         </is>
       </c>
     </row>
@@ -6911,7 +6911,7 @@
       </c>
       <c r="F170" t="inlineStr">
         <is>
-          <t>1:M56,1:M57,1:M58,1:M59,1:M60,1:M61,1:M62,1:M63</t>
+          <t>1:5G-M56,1:5G-M57,1:5G-M58,1:5G-M59,1:5G-M60,1:5G-M61,1:5G-M62,1:5G-M63</t>
         </is>
       </c>
     </row>
@@ -6955,7 +6955,7 @@
       </c>
       <c r="F172" t="inlineStr">
         <is>
-          <t>1:M56,1:M57,1:M58,1:M59,1:M60,1:M61,1:M62,1:M63</t>
+          <t>1:5G-M56,1:5G-M57,1:5G-M58,1:5G-M59,1:5G-M60,1:5G-M61,1:5G-M62,1:5G-M63</t>
         </is>
       </c>
     </row>
@@ -6999,7 +6999,7 @@
       </c>
       <c r="F174" t="inlineStr">
         <is>
-          <t>1:M56,1:M57,1:M58,1:M59,1:M60,1:M61,1:M62,1:M63</t>
+          <t>1:5G-M56,1:5G-M57,1:5G-M58,1:5G-M59,1:5G-M60,1:5G-M61,1:5G-M62,1:5G-M63</t>
         </is>
       </c>
     </row>
@@ -7043,7 +7043,7 @@
       </c>
       <c r="F176" t="inlineStr">
         <is>
-          <t>1:M56,1:M57,1:M58,1:M59,1:M60,1:M61,1:M62,1:M63</t>
+          <t>1:5G-M56,1:5G-M57,1:5G-M58,1:5G-M59,1:5G-M60,1:5G-M61,1:5G-M62,1:5G-M63</t>
         </is>
       </c>
     </row>
@@ -7087,7 +7087,7 @@
       </c>
       <c r="F178" t="inlineStr">
         <is>
-          <t>1:M56,1:M57,1:M58,1:M59,1:M60,1:M61,1:M62,1:M63</t>
+          <t>1:5G-M56,1:5G-M57,1:5G-M58,1:5G-M59,1:5G-M60,1:5G-M61,1:5G-M62,1:5G-M63</t>
         </is>
       </c>
     </row>
@@ -7131,7 +7131,7 @@
       </c>
       <c r="F180" t="inlineStr">
         <is>
-          <t>1:M56,1:M57,1:M58,1:M59,1:M60,1:M61,1:M62,1:M63</t>
+          <t>1:5G-M56,1:5G-M57,1:5G-M58,1:5G-M59,1:5G-M60,1:5G-M61,1:5G-M62,1:5G-M63</t>
         </is>
       </c>
     </row>
@@ -7175,7 +7175,7 @@
       </c>
       <c r="F182" t="inlineStr">
         <is>
-          <t>1:M56,1:M57,1:M58,1:M59,1:M60,1:M61,1:M62,1:M63</t>
+          <t>1:5G-M56,1:5G-M57,1:5G-M58,1:5G-M59,1:5G-M60,1:5G-M61,1:5G-M62,1:5G-M63</t>
         </is>
       </c>
     </row>
@@ -7219,7 +7219,7 @@
       </c>
       <c r="F184" t="inlineStr">
         <is>
-          <t>1:M56,1:M57,1:M58,1:M59,1:M60,1:M61,1:M62,1:M63</t>
+          <t>1:5G-M56,1:5G-M57,1:5G-M58,1:5G-M59,1:5G-M60,1:5G-M61,1:5G-M62,1:5G-M63</t>
         </is>
       </c>
     </row>
@@ -7263,7 +7263,7 @@
       </c>
       <c r="F186" t="inlineStr">
         <is>
-          <t>1:M56,1:M57,1:M58,1:M59,1:M60,1:M61,1:M62,1:M63</t>
+          <t>1:5G-M56,1:5G-M57,1:5G-M58,1:5G-M59,1:5G-M60,1:5G-M61,1:5G-M62,1:5G-M63</t>
         </is>
       </c>
     </row>
@@ -7307,7 +7307,7 @@
       </c>
       <c r="F188" t="inlineStr">
         <is>
-          <t>1:M56,1:M57,1:M58,1:M59,1:M60,1:M61,1:M62,1:M63</t>
+          <t>1:5G-M56,1:5G-M57,1:5G-M58,1:5G-M59,1:5G-M60,1:5G-M61,1:5G-M62,1:5G-M63</t>
         </is>
       </c>
     </row>
@@ -7351,7 +7351,7 @@
       </c>
       <c r="F190" t="inlineStr">
         <is>
-          <t>1:M56,1:M57,1:M58,1:M59,1:M60,1:M61,1:M62,1:M63</t>
+          <t>1:5G-M56,1:5G-M57,1:5G-M58,1:5G-M59,1:5G-M60,1:5G-M61,1:5G-M62,1:5G-M63</t>
         </is>
       </c>
     </row>
@@ -7395,7 +7395,7 @@
       </c>
       <c r="F192" t="inlineStr">
         <is>
-          <t>1:M56,1:M57,1:M58,1:M59,1:M60,1:M61,1:M62,1:M63</t>
+          <t>1:5G-M56,1:5G-M57,1:5G-M58,1:5G-M59,1:5G-M60,1:5G-M61,1:5G-M62,1:5G-M63</t>
         </is>
       </c>
     </row>
@@ -7439,7 +7439,7 @@
       </c>
       <c r="F194" t="inlineStr">
         <is>
-          <t>1:M56,1:M57,1:M58,1:M59,1:M60,1:M61,1:M62,1:M63</t>
+          <t>1:5G-M56,1:5G-M57,1:5G-M58,1:5G-M59,1:5G-M60,1:5G-M61,1:5G-M62,1:5G-M63</t>
         </is>
       </c>
     </row>
@@ -7484,7 +7484,7 @@
       </c>
       <c r="F196" t="inlineStr">
         <is>
-          <t>1:M56,1:M57,1:M58,1:M59,1:M60,1:M61,1:M62,1:M63</t>
+          <t>1:5G-M56,1:5G-M57,1:5G-M58,1:5G-M59,1:5G-M60,1:5G-M61,1:5G-M62,1:5G-M63</t>
         </is>
       </c>
     </row>
@@ -7528,7 +7528,7 @@
       </c>
       <c r="F198" t="inlineStr">
         <is>
-          <t>1:M56,1:M57,1:M58,1:M59,1:M60,1:M61,1:M62,1:M63</t>
+          <t>1:5G-M56,1:5G-M57,1:5G-M58,1:5G-M59,1:5G-M60,1:5G-M61,1:5G-M62,1:5G-M63</t>
         </is>
       </c>
     </row>
@@ -7572,7 +7572,7 @@
       </c>
       <c r="F200" t="inlineStr">
         <is>
-          <t>1:M56,1:M57,1:M58,1:M59,1:M60,1:M61,1:M62,1:M63</t>
+          <t>1:5G-M56,1:5G-M57,1:5G-M58,1:5G-M59,1:5G-M60,1:5G-M61,1:5G-M62,1:5G-M63</t>
         </is>
       </c>
     </row>
@@ -7616,7 +7616,7 @@
       </c>
       <c r="F202" t="inlineStr">
         <is>
-          <t>1:M56,1:M57,1:M58,1:M59,1:M60,1:M61,1:M62,1:M63</t>
+          <t>1:5G-M56,1:5G-M57,1:5G-M58,1:5G-M59,1:5G-M60,1:5G-M61,1:5G-M62,1:5G-M63</t>
         </is>
       </c>
     </row>
@@ -7660,7 +7660,7 @@
       </c>
       <c r="F204" t="inlineStr">
         <is>
-          <t>1:M56,1:M57,1:M58,1:M59,1:M60,1:M61,1:M62,1:M63</t>
+          <t>1:5G-M56,1:5G-M57,1:5G-M58,1:5G-M59,1:5G-M60,1:5G-M61,1:5G-M62,1:5G-M63</t>
         </is>
       </c>
     </row>
@@ -7704,7 +7704,7 @@
       </c>
       <c r="F206" t="inlineStr">
         <is>
-          <t>1:M56,1:M57,1:M58,1:M59,1:M60,1:M61,1:M62,1:M63</t>
+          <t>1:5G-M56,1:5G-M57,1:5G-M58,1:5G-M59,1:5G-M60,1:5G-M61,1:5G-M62,1:5G-M63</t>
         </is>
       </c>
     </row>
@@ -7749,7 +7749,7 @@
       </c>
       <c r="F208" t="inlineStr">
         <is>
-          <t>1:M56,1:M57,1:M58,1:M59,1:M60,1:M61,1:M62,1:M63</t>
+          <t>1:5G-M56,1:5G-M57,1:5G-M58,1:5G-M59,1:5G-M60,1:5G-M61,1:5G-M62,1:5G-M63</t>
         </is>
       </c>
     </row>
@@ -7793,7 +7793,7 @@
       </c>
       <c r="F210" t="inlineStr">
         <is>
-          <t>1:M56,1:M57,1:M58,1:M59,1:M60,1:M61,1:M62,1:M63</t>
+          <t>1:5G-M56,1:5G-M57,1:5G-M58,1:5G-M59,1:5G-M60,1:5G-M61,1:5G-M62,1:5G-M63</t>
         </is>
       </c>
     </row>
@@ -7837,7 +7837,7 @@
       </c>
       <c r="F212" t="inlineStr">
         <is>
-          <t>1:M56,1:M57,1:M58,1:M59,1:M60,1:M61,1:M62,1:M63</t>
+          <t>1:5G-M56,1:5G-M57,1:5G-M58,1:5G-M59,1:5G-M60,1:5G-M61,1:5G-M62,1:5G-M63</t>
         </is>
       </c>
     </row>
@@ -7881,7 +7881,7 @@
       </c>
       <c r="F214" t="inlineStr">
         <is>
-          <t>1:M56,1:M57,1:M58,1:M59,1:M60,1:M61,1:M62,1:M63</t>
+          <t>1:5G-M56,1:5G-M57,1:5G-M58,1:5G-M59,1:5G-M60,1:5G-M61,1:5G-M62,1:5G-M63</t>
         </is>
       </c>
     </row>
@@ -7925,7 +7925,7 @@
       </c>
       <c r="F216" t="inlineStr">
         <is>
-          <t>1:M56,1:M57,1:M58,1:M59,1:M60,1:M61,1:M62,1:M63</t>
+          <t>1:5G-M56,1:5G-M57,1:5G-M58,1:5G-M59,1:5G-M60,1:5G-M61,1:5G-M62,1:5G-M63</t>
         </is>
       </c>
     </row>
@@ -7969,7 +7969,7 @@
       </c>
       <c r="F218" t="inlineStr">
         <is>
-          <t>1:M56,1:M57,1:M58,1:M59,1:M60,1:M61,1:M62,1:M63</t>
+          <t>1:5G-M56,1:5G-M57,1:5G-M58,1:5G-M59,1:5G-M60,1:5G-M61,1:5G-M62,1:5G-M63</t>
         </is>
       </c>
     </row>
@@ -8013,7 +8013,7 @@
       </c>
       <c r="F220" t="inlineStr">
         <is>
-          <t>1:M56,1:M57,1:M58,1:M59,1:M60,1:M61,1:M62,1:M63</t>
+          <t>1:5G-M56,1:5G-M57,1:5G-M58,1:5G-M59,1:5G-M60,1:5G-M61,1:5G-M62,1:5G-M63</t>
         </is>
       </c>
     </row>
@@ -8057,7 +8057,7 @@
       </c>
       <c r="F222" t="inlineStr">
         <is>
-          <t>1:M56,1:M57,1:M58,1:M59,1:M60,1:M61,1:M62,1:M63</t>
+          <t>1:5G-M56,1:5G-M57,1:5G-M58,1:5G-M59,1:5G-M60,1:5G-M61,1:5G-M62,1:5G-M63</t>
         </is>
       </c>
     </row>
@@ -8101,7 +8101,7 @@
       </c>
       <c r="F224" t="inlineStr">
         <is>
-          <t>1:M56,1:M57,1:M58,1:M59,1:M60,1:M61,1:M62,1:M63</t>
+          <t>1:5G-M56,1:5G-M57,1:5G-M58,1:5G-M59,1:5G-M60,1:5G-M61,1:5G-M62,1:5G-M63</t>
         </is>
       </c>
     </row>
@@ -8145,7 +8145,7 @@
       </c>
       <c r="F226" t="inlineStr">
         <is>
-          <t>1:M56,1:M57,1:M58,1:M59,1:M60,1:M61,1:M62,1:M63</t>
+          <t>1:5G-M56,1:5G-M57,1:5G-M58,1:5G-M59,1:5G-M60,1:5G-M61,1:5G-M62,1:5G-M63</t>
         </is>
       </c>
     </row>
@@ -8191,7 +8191,7 @@
       </c>
       <c r="F228" t="inlineStr">
         <is>
-          <t>1:M56,1:M57,1:M58,1:M59,1:M60,1:M61,1:M62,1:M63</t>
+          <t>1:5G-M56,1:5G-M57,1:5G-M58,1:5G-M59,1:5G-M60,1:5G-M61,1:5G-M62,1:5G-M63</t>
         </is>
       </c>
     </row>
@@ -8235,7 +8235,7 @@
       </c>
       <c r="F230" t="inlineStr">
         <is>
-          <t>1:M56,1:M57,1:M58,1:M59,1:M60,1:M61,1:M62,1:M63</t>
+          <t>1:5G-M56,1:5G-M57,1:5G-M58,1:5G-M59,1:5G-M60,1:5G-M61,1:5G-M62,1:5G-M63</t>
         </is>
       </c>
     </row>
@@ -8279,7 +8279,7 @@
       </c>
       <c r="F232" t="inlineStr">
         <is>
-          <t>1:M56,1:M57,1:M58,1:M59,1:M60,1:M61,1:M62,1:M63</t>
+          <t>1:5G-M56,1:5G-M57,1:5G-M58,1:5G-M59,1:5G-M60,1:5G-M61,1:5G-M62,1:5G-M63</t>
         </is>
       </c>
     </row>
@@ -8323,7 +8323,7 @@
       </c>
       <c r="F234" t="inlineStr">
         <is>
-          <t>1:M56,1:M57,1:M58,1:M59,1:M60,1:M61,1:M62,1:M63</t>
+          <t>1:5G-M56,1:5G-M57,1:5G-M58,1:5G-M59,1:5G-M60,1:5G-M61,1:5G-M62,1:5G-M63</t>
         </is>
       </c>
     </row>
@@ -8367,7 +8367,7 @@
       </c>
       <c r="F236" t="inlineStr">
         <is>
-          <t>1:M56,1:M57,1:M58,1:M59,1:M60,1:M61,1:M62,1:M63</t>
+          <t>1:5G-M56,1:5G-M57,1:5G-M58,1:5G-M59,1:5G-M60,1:5G-M61,1:5G-M62,1:5G-M63</t>
         </is>
       </c>
     </row>
@@ -8411,7 +8411,7 @@
       </c>
       <c r="F238" t="inlineStr">
         <is>
-          <t>1:M56,1:M57,1:M58,1:M59,1:M60,1:M61,1:M62,1:M63</t>
+          <t>1:5G-M56,1:5G-M57,1:5G-M58,1:5G-M59,1:5G-M60,1:5G-M61,1:5G-M62,1:5G-M63</t>
         </is>
       </c>
     </row>
@@ -8457,7 +8457,7 @@
       </c>
       <c r="F240" t="inlineStr">
         <is>
-          <t>1:M56,1:M57,1:M58,1:M59,1:M60,1:M61,1:M62,1:M63</t>
+          <t>1:5G-M56,1:5G-M57,1:5G-M58,1:5G-M59,1:5G-M60,1:5G-M61,1:5G-M62,1:5G-M63</t>
         </is>
       </c>
     </row>
@@ -8501,7 +8501,7 @@
       </c>
       <c r="F242" t="inlineStr">
         <is>
-          <t>1:M56,1:M57,1:M58,1:M59,1:M60,1:M61,1:M62,1:M63</t>
+          <t>1:5G-M56,1:5G-M57,1:5G-M58,1:5G-M59,1:5G-M60,1:5G-M61,1:5G-M62,1:5G-M63</t>
         </is>
       </c>
     </row>
@@ -8545,7 +8545,7 @@
       </c>
       <c r="F244" t="inlineStr">
         <is>
-          <t>1:M56,1:M57,1:M58,1:M59,1:M60,1:M61,1:M62,1:M63</t>
+          <t>1:5G-M56,1:5G-M57,1:5G-M58,1:5G-M59,1:5G-M60,1:5G-M61,1:5G-M62,1:5G-M63</t>
         </is>
       </c>
     </row>
@@ -8589,7 +8589,7 @@
       </c>
       <c r="F246" t="inlineStr">
         <is>
-          <t>1:M56,1:M57,1:M58,1:M59,1:M60,1:M61,1:M62,1:M63</t>
+          <t>1:5G-M56,1:5G-M57,1:5G-M58,1:5G-M59,1:5G-M60,1:5G-M61,1:5G-M62,1:5G-M63</t>
         </is>
       </c>
     </row>
@@ -8633,7 +8633,7 @@
       </c>
       <c r="F248" t="inlineStr">
         <is>
-          <t>1:M56,1:M57,1:M58,1:M59,1:M60,1:M61,1:M62,1:M63</t>
+          <t>1:5G-M56,1:5G-M57,1:5G-M58,1:5G-M59,1:5G-M60,1:5G-M61,1:5G-M62,1:5G-M63</t>
         </is>
       </c>
     </row>
@@ -8677,7 +8677,7 @@
       </c>
       <c r="F250" t="inlineStr">
         <is>
-          <t>1:M56,1:M57,1:M58,1:M59,1:M60,1:M61,1:M62,1:M63</t>
+          <t>1:5G-M56,1:5G-M57,1:5G-M58,1:5G-M59,1:5G-M60,1:5G-M61,1:5G-M62,1:5G-M63</t>
         </is>
       </c>
     </row>
@@ -8722,7 +8722,7 @@
       </c>
       <c r="F252" t="inlineStr">
         <is>
-          <t>1:M56,1:M57,1:M58,1:M59,1:M60,1:M61,1:M62,1:M63</t>
+          <t>1:5G-M56,1:5G-M57,1:5G-M58,1:5G-M59,1:5G-M60,1:5G-M61,1:5G-M62,1:5G-M63</t>
         </is>
       </c>
     </row>
@@ -8767,7 +8767,7 @@
       </c>
       <c r="F254" t="inlineStr">
         <is>
-          <t>1:M56,1:M57,1:M58,1:M59,1:M60,1:M61,1:M62,1:M63</t>
+          <t>1:5G-M56,1:5G-M57,1:5G-M58,1:5G-M59,1:5G-M60,1:5G-M61,1:5G-M62,1:5G-M63</t>
         </is>
       </c>
     </row>
@@ -8811,7 +8811,7 @@
       </c>
       <c r="F256" t="inlineStr">
         <is>
-          <t>1:M56,1:M57,1:M58,1:M59,1:M60,1:M61,1:M62,1:M63</t>
+          <t>1:5G-M56,1:5G-M57,1:5G-M58,1:5G-M59,1:5G-M60,1:5G-M61,1:5G-M62,1:5G-M63</t>
         </is>
       </c>
     </row>
@@ -8857,7 +8857,7 @@
       </c>
       <c r="F258" t="inlineStr">
         <is>
-          <t>1:M56,1:M57,1:M58,1:M59,1:M60,1:M61,1:M62,1:M63</t>
+          <t>1:5G-M56,1:5G-M57,1:5G-M58,1:5G-M59,1:5G-M60,1:5G-M61,1:5G-M62,1:5G-M63</t>
         </is>
       </c>
     </row>
@@ -8904,7 +8904,7 @@
       </c>
       <c r="F260" t="inlineStr">
         <is>
-          <t>1:M56,1:M57,1:M58,1:M59,1:M60,1:M61,1:M62,1:M63</t>
+          <t>1:5G-M56,1:5G-M57,1:5G-M58,1:5G-M59,1:5G-M60,1:5G-M61,1:5G-M62,1:5G-M63</t>
         </is>
       </c>
     </row>
@@ -8956,7 +8956,7 @@
       </c>
       <c r="F262" t="inlineStr">
         <is>
-          <t>1:M56,1:M57,1:M58,1:M59,1:M60,1:M61,1:M62,1:M63</t>
+          <t>1:5G-M56,1:5G-M57,1:5G-M58,1:5G-M59,1:5G-M60,1:5G-M61,1:5G-M62,1:5G-M63</t>
         </is>
       </c>
     </row>
@@ -9005,7 +9005,7 @@
       </c>
       <c r="F264" t="inlineStr">
         <is>
-          <t>1:M56,1:M57,1:M58,1:M59,1:M60,1:M61,1:M62,1:M63</t>
+          <t>1:5G-M56,1:5G-M57,1:5G-M58,1:5G-M59,1:5G-M60,1:5G-M61,1:5G-M62,1:5G-M63</t>
         </is>
       </c>
     </row>
@@ -9054,7 +9054,7 @@
       </c>
       <c r="F266" t="inlineStr">
         <is>
-          <t>1:M56,1:M57,1:M58,1:M59,1:M60,1:M61,1:M62,1:M63</t>
+          <t>1:5G-M56,1:5G-M57,1:5G-M58,1:5G-M59,1:5G-M60,1:5G-M61,1:5G-M62,1:5G-M63</t>
         </is>
       </c>
     </row>
@@ -9106,7 +9106,7 @@
       </c>
       <c r="F268" t="inlineStr">
         <is>
-          <t>1:M56,1:M57,1:M58,1:M59,1:M60,1:M61,1:M62,1:M63</t>
+          <t>1:5G-M56,1:5G-M57,1:5G-M58,1:5G-M59,1:5G-M60,1:5G-M61,1:5G-M62,1:5G-M63</t>
         </is>
       </c>
     </row>
@@ -9156,7 +9156,7 @@
       </c>
       <c r="F270" t="inlineStr">
         <is>
-          <t>1:M56,1:M57,1:M58,1:M59,1:M60,1:M61,1:M62,1:M63</t>
+          <t>1:5G-M56,1:5G-M57,1:5G-M58,1:5G-M59,1:5G-M60,1:5G-M61,1:5G-M62,1:5G-M63</t>
         </is>
       </c>
     </row>
@@ -9204,7 +9204,7 @@
       </c>
       <c r="F272" t="inlineStr">
         <is>
-          <t>1:M56,1:M57,1:M58,1:M59,1:M60,1:M61,1:M62,1:M63</t>
+          <t>1:5G-M56,1:5G-M57,1:5G-M58,1:5G-M59,1:5G-M60,1:5G-M61,1:5G-M62,1:5G-M63</t>
         </is>
       </c>
     </row>
@@ -9249,7 +9249,7 @@
       </c>
       <c r="F274" t="inlineStr">
         <is>
-          <t>1:M56,1:M57,1:M58,1:M59,1:M60,1:M61,1:M62,1:M63</t>
+          <t>1:5G-M56,1:5G-M57,1:5G-M58,1:5G-M59,1:5G-M60,1:5G-M61,1:5G-M62,1:5G-M63</t>
         </is>
       </c>
     </row>
@@ -9302,7 +9302,7 @@
       </c>
       <c r="F276" t="inlineStr">
         <is>
-          <t>1:M56,1:M57,1:M58,1:M59,1:M60,1:M61,1:M62,1:M63</t>
+          <t>1:5G-M56,1:5G-M57,1:5G-M58,1:5G-M59,1:5G-M60,1:5G-M61,1:5G-M62,1:5G-M63</t>
         </is>
       </c>
     </row>
@@ -9349,7 +9349,7 @@
       </c>
       <c r="F278" t="inlineStr">
         <is>
-          <t>1:M56,1:M57,1:M58,1:M59,1:M60,1:M61,1:M62,1:M63</t>
+          <t>1:5G-M56,1:5G-M57,1:5G-M58,1:5G-M59,1:5G-M60,1:5G-M61,1:5G-M62,1:5G-M63</t>
         </is>
       </c>
     </row>
@@ -9393,7 +9393,7 @@
       </c>
       <c r="F280" t="inlineStr">
         <is>
-          <t>1:M56,1:M57,1:M58,1:M59,1:M60,1:M61,1:M62,1:M63</t>
+          <t>1:5G-M56,1:5G-M57,1:5G-M58,1:5G-M59,1:5G-M60,1:5G-M61,1:5G-M62,1:5G-M63</t>
         </is>
       </c>
     </row>
@@ -9437,7 +9437,7 @@
       </c>
       <c r="F282" t="inlineStr">
         <is>
-          <t>1:M56,1:M57,1:M58,1:M59,1:M60,1:M61,1:M62,1:M63</t>
+          <t>1:5G-M56,1:5G-M57,1:5G-M58,1:5G-M59,1:5G-M60,1:5G-M61,1:5G-M62,1:5G-M63</t>
         </is>
       </c>
     </row>
@@ -9482,7 +9482,7 @@
       </c>
       <c r="F284" t="inlineStr">
         <is>
-          <t>1:M56,1:M57,1:M58,1:M59,1:M60,1:M61,1:M62,1:M63</t>
+          <t>1:5G-M56,1:5G-M57,1:5G-M58,1:5G-M59,1:5G-M60,1:5G-M61,1:5G-M62,1:5G-M63</t>
         </is>
       </c>
     </row>
@@ -9528,7 +9528,7 @@
       </c>
       <c r="F286" t="inlineStr">
         <is>
-          <t>1:M56,1:M57,1:M58,1:M59,1:M60,1:M61,1:M62,1:M63</t>
+          <t>1:5G-M56,1:5G-M57,1:5G-M58,1:5G-M59,1:5G-M60,1:5G-M61,1:5G-M62,1:5G-M63</t>
         </is>
       </c>
     </row>
@@ -9574,7 +9574,7 @@
       </c>
       <c r="F288" t="inlineStr">
         <is>
-          <t>1:M56,1:M57,1:M58,1:M59,1:M60,1:M61,1:M62,1:M63</t>
+          <t>1:5G-M56,1:5G-M57,1:5G-M58,1:5G-M59,1:5G-M60,1:5G-M61,1:5G-M62,1:5G-M63</t>
         </is>
       </c>
     </row>
@@ -9626,7 +9626,7 @@
       </c>
       <c r="F290" t="inlineStr">
         <is>
-          <t>1:M56,1:M57,1:M58,1:M59,1:M60,1:M61,1:M62,1:M63</t>
+          <t>1:5G-M56,1:5G-M57,1:5G-M58,1:5G-M59,1:5G-M60,1:5G-M61,1:5G-M62,1:5G-M63</t>
         </is>
       </c>
     </row>
@@ -9671,7 +9671,7 @@
       </c>
       <c r="F292" t="inlineStr">
         <is>
-          <t>1:M56,1:M57,1:M58,1:M59,1:M60,1:M61,1:M62,1:M63</t>
+          <t>1:5G-M56,1:5G-M57,1:5G-M58,1:5G-M59,1:5G-M60,1:5G-M61,1:5G-M62,1:5G-M63</t>
         </is>
       </c>
     </row>
@@ -9715,7 +9715,7 @@
       </c>
       <c r="F294" t="inlineStr">
         <is>
-          <t>1:M56,1:M57,1:M58,1:M59,1:M60,1:M61,1:M62,1:M63</t>
+          <t>1:5G-M56,1:5G-M57,1:5G-M58,1:5G-M59,1:5G-M60,1:5G-M61,1:5G-M62,1:5G-M63</t>
         </is>
       </c>
     </row>
@@ -9760,7 +9760,7 @@
       </c>
       <c r="F296" t="inlineStr">
         <is>
-          <t>1:M56,1:M57,1:M58,1:M59,1:M60,1:M61,1:M62,1:M63</t>
+          <t>1:5G-M56,1:5G-M57,1:5G-M58,1:5G-M59,1:5G-M60,1:5G-M61,1:5G-M62,1:5G-M63</t>
         </is>
       </c>
     </row>
@@ -9807,7 +9807,7 @@
       </c>
       <c r="F298" t="inlineStr">
         <is>
-          <t>1:M56,1:M57,1:M58,1:M59,1:M60,1:M61,1:M62,1:M63</t>
+          <t>1:5G-M56,1:5G-M57,1:5G-M58,1:5G-M59,1:5G-M60,1:5G-M61,1:5G-M62,1:5G-M63</t>
         </is>
       </c>
     </row>
@@ -9851,7 +9851,7 @@
       </c>
       <c r="F300" t="inlineStr">
         <is>
-          <t>1:M56,1:M57,1:M58,1:M59,1:M60,1:M61,1:M62,1:M63</t>
+          <t>1:5G-M56,1:5G-M57,1:5G-M58,1:5G-M59,1:5G-M60,1:5G-M61,1:5G-M62,1:5G-M63</t>
         </is>
       </c>
     </row>
@@ -9895,7 +9895,7 @@
       </c>
       <c r="F302" t="inlineStr">
         <is>
-          <t>1:M56,1:M57,1:M58,1:M59,1:M60,1:M61,1:M62,1:M63</t>
+          <t>1:5G-M56,1:5G-M57,1:5G-M58,1:5G-M59,1:5G-M60,1:5G-M61,1:5G-M62,1:5G-M63</t>
         </is>
       </c>
     </row>
@@ -9939,7 +9939,7 @@
       </c>
       <c r="F304" t="inlineStr">
         <is>
-          <t>1:M56,1:M57,1:M58,1:M59,1:M60,1:M61,1:M62,1:M63</t>
+          <t>1:5G-M56,1:5G-M57,1:5G-M58,1:5G-M59,1:5G-M60,1:5G-M61,1:5G-M62,1:5G-M63</t>
         </is>
       </c>
     </row>
@@ -9983,7 +9983,7 @@
       </c>
       <c r="F306" t="inlineStr">
         <is>
-          <t>1:M56,1:M57,1:M58,1:M59,1:M60,1:M61,1:M62,1:M63</t>
+          <t>1:5G-M56,1:5G-M57,1:5G-M58,1:5G-M59,1:5G-M60,1:5G-M61,1:5G-M62,1:5G-M63</t>
         </is>
       </c>
     </row>
@@ -10028,7 +10028,7 @@
       </c>
       <c r="F308" t="inlineStr">
         <is>
-          <t>1:M56,1:M57,1:M58,1:M59,1:M60,1:M61,1:M62,1:M63</t>
+          <t>1:5G-M56,1:5G-M57,1:5G-M58,1:5G-M59,1:5G-M60,1:5G-M61,1:5G-M62,1:5G-M63</t>
         </is>
       </c>
     </row>
@@ -10079,7 +10079,7 @@
       </c>
       <c r="F310" t="inlineStr">
         <is>
-          <t>1:M56,1:M57,1:M58,1:M59,1:M60,1:M61,1:M62,1:M63</t>
+          <t>1:5G-M56,1:5G-M57,1:5G-M58,1:5G-M59,1:5G-M60,1:5G-M61,1:5G-M62,1:5G-M63</t>
         </is>
       </c>
     </row>
@@ -10123,7 +10123,7 @@
       </c>
       <c r="F312" t="inlineStr">
         <is>
-          <t>1:M56,1:M57,1:M58,1:M59,1:M60,1:M61,1:M62,1:M63</t>
+          <t>1:5G-M56,1:5G-M57,1:5G-M58,1:5G-M59,1:5G-M60,1:5G-M61,1:5G-M62,1:5G-M63</t>
         </is>
       </c>
     </row>
@@ -10167,7 +10167,7 @@
       </c>
       <c r="F314" t="inlineStr">
         <is>
-          <t>1:M56,1:M57,1:M58,1:M59,1:M60,1:M61,1:M62,1:M63</t>
+          <t>1:5G-M56,1:5G-M57,1:5G-M58,1:5G-M59,1:5G-M60,1:5G-M61,1:5G-M62,1:5G-M63</t>
         </is>
       </c>
     </row>
@@ -10211,7 +10211,7 @@
       </c>
       <c r="F316" t="inlineStr">
         <is>
-          <t>1:M56,1:M57,1:M58,1:M59,1:M60,1:M61,1:M62,1:M63</t>
+          <t>1:5G-M56,1:5G-M57,1:5G-M58,1:5G-M59,1:5G-M60,1:5G-M61,1:5G-M62,1:5G-M63</t>
         </is>
       </c>
     </row>
@@ -10255,7 +10255,7 @@
       </c>
       <c r="F318" t="inlineStr">
         <is>
-          <t>1:M56,1:M57,1:M58,1:M59,1:M60,1:M61,1:M62,1:M63</t>
+          <t>1:5G-M56,1:5G-M57,1:5G-M58,1:5G-M59,1:5G-M60,1:5G-M61,1:5G-M62,1:5G-M63</t>
         </is>
       </c>
     </row>
@@ -10299,7 +10299,7 @@
       </c>
       <c r="F320" t="inlineStr">
         <is>
-          <t>1:M56,1:M57,1:M58,1:M59,1:M60,1:M61,1:M62,1:M63</t>
+          <t>1:5G-M56,1:5G-M57,1:5G-M58,1:5G-M59,1:5G-M60,1:5G-M61,1:5G-M62,1:5G-M63</t>
         </is>
       </c>
     </row>
@@ -10365,7 +10365,7 @@
       </c>
       <c r="F323" t="inlineStr">
         <is>
-          <t>1:M64,1:M65,1:M66,1:M67,1:M68,1:M69</t>
+          <t>1:5G-M64,1:5G-M65,1:5G-M66,1:5G-M67,1:5G-M68,1:5G-M69</t>
         </is>
       </c>
     </row>
@@ -10409,7 +10409,7 @@
       </c>
       <c r="F325" t="inlineStr">
         <is>
-          <t>1:M64,1:M65,1:M66,1:M67,1:M68,1:M69</t>
+          <t>1:5G-M64,1:5G-M65,1:5G-M66,1:5G-M67,1:5G-M68,1:5G-M69</t>
         </is>
       </c>
     </row>
@@ -10453,7 +10453,7 @@
       </c>
       <c r="F327" t="inlineStr">
         <is>
-          <t>1:M64,1:M65,1:M66,1:M67,1:M68,1:M69</t>
+          <t>1:5G-M64,1:5G-M65,1:5G-M66,1:5G-M67,1:5G-M68,1:5G-M69</t>
         </is>
       </c>
     </row>
@@ -10497,7 +10497,7 @@
       </c>
       <c r="F329" t="inlineStr">
         <is>
-          <t>1:M64,1:M65,1:M66,1:M67,1:M68,1:M69</t>
+          <t>1:5G-M64,1:5G-M65,1:5G-M66,1:5G-M67,1:5G-M68,1:5G-M69</t>
         </is>
       </c>
     </row>
@@ -10541,7 +10541,7 @@
       </c>
       <c r="F331" t="inlineStr">
         <is>
-          <t>1:M64,1:M65,1:M66,1:M67,1:M68,1:M69</t>
+          <t>1:5G-M64,1:5G-M65,1:5G-M66,1:5G-M67,1:5G-M68,1:5G-M69</t>
         </is>
       </c>
     </row>
@@ -10585,7 +10585,7 @@
       </c>
       <c r="F333" t="inlineStr">
         <is>
-          <t>1:M64,1:M65,1:M66,1:M67,1:M68,1:M69</t>
+          <t>1:5G-M64,1:5G-M65,1:5G-M66,1:5G-M67,1:5G-M68,1:5G-M69</t>
         </is>
       </c>
     </row>
@@ -10629,7 +10629,7 @@
       </c>
       <c r="F335" t="inlineStr">
         <is>
-          <t>1:M64,1:M65,1:M66,1:M67,1:M68,1:M69</t>
+          <t>1:5G-M64,1:5G-M65,1:5G-M66,1:5G-M67,1:5G-M68,1:5G-M69</t>
         </is>
       </c>
     </row>
@@ -10673,7 +10673,7 @@
       </c>
       <c r="F337" t="inlineStr">
         <is>
-          <t>1:M64,1:M65,1:M66,1:M67,1:M68,1:M69</t>
+          <t>1:5G-M64,1:5G-M65,1:5G-M66,1:5G-M67,1:5G-M68,1:5G-M69</t>
         </is>
       </c>
     </row>
@@ -10717,7 +10717,7 @@
       </c>
       <c r="F339" t="inlineStr">
         <is>
-          <t>1:M64,1:M65,1:M66,1:M67,1:M68,1:M69</t>
+          <t>1:5G-M64,1:5G-M65,1:5G-M66,1:5G-M67,1:5G-M68,1:5G-M69</t>
         </is>
       </c>
     </row>
@@ -10761,7 +10761,7 @@
       </c>
       <c r="F341" t="inlineStr">
         <is>
-          <t>1:M64,1:M65,1:M66,1:M67,1:M68,1:M69</t>
+          <t>1:5G-M64,1:5G-M65,1:5G-M66,1:5G-M67,1:5G-M68,1:5G-M69</t>
         </is>
       </c>
     </row>
@@ -10805,7 +10805,7 @@
       </c>
       <c r="F343" t="inlineStr">
         <is>
-          <t>1:M64,1:M65,1:M66,1:M67,1:M68,1:M69</t>
+          <t>1:5G-M64,1:5G-M65,1:5G-M66,1:5G-M67,1:5G-M68,1:5G-M69</t>
         </is>
       </c>
     </row>
@@ -10849,7 +10849,7 @@
       </c>
       <c r="F345" t="inlineStr">
         <is>
-          <t>1:M64,1:M65,1:M66,1:M67,1:M68,1:M69</t>
+          <t>1:5G-M64,1:5G-M65,1:5G-M66,1:5G-M67,1:5G-M68,1:5G-M69</t>
         </is>
       </c>
     </row>
@@ -10893,7 +10893,7 @@
       </c>
       <c r="F347" t="inlineStr">
         <is>
-          <t>1:M64,1:M65,1:M66,1:M67,1:M68,1:M69</t>
+          <t>1:5G-M64,1:5G-M65,1:5G-M66,1:5G-M67,1:5G-M68,1:5G-M69</t>
         </is>
       </c>
     </row>
@@ -10937,7 +10937,7 @@
       </c>
       <c r="F349" t="inlineStr">
         <is>
-          <t>1:M64,1:M65,1:M66,1:M67,1:M68,1:M69</t>
+          <t>1:5G-M64,1:5G-M65,1:5G-M66,1:5G-M67,1:5G-M68,1:5G-M69</t>
         </is>
       </c>
     </row>
@@ -10981,7 +10981,7 @@
       </c>
       <c r="F351" t="inlineStr">
         <is>
-          <t>1:M64,1:M65,1:M66,1:M67,1:M68,1:M69</t>
+          <t>1:5G-M64,1:5G-M65,1:5G-M66,1:5G-M67,1:5G-M68,1:5G-M69</t>
         </is>
       </c>
     </row>
@@ -11025,7 +11025,7 @@
       </c>
       <c r="F353" t="inlineStr">
         <is>
-          <t>1:M64,1:M65,1:M66,1:M67,1:M68,1:M69</t>
+          <t>1:5G-M64,1:5G-M65,1:5G-M66,1:5G-M67,1:5G-M68,1:5G-M69</t>
         </is>
       </c>
     </row>
@@ -11069,7 +11069,7 @@
       </c>
       <c r="F355" t="inlineStr">
         <is>
-          <t>1:M64,1:M65,1:M66,1:M67,1:M68,1:M69</t>
+          <t>1:5G-M64,1:5G-M65,1:5G-M66,1:5G-M67,1:5G-M68,1:5G-M69</t>
         </is>
       </c>
     </row>
@@ -11114,7 +11114,7 @@
       </c>
       <c r="F357" t="inlineStr">
         <is>
-          <t>1:M64,1:M65,1:M66,1:M67,1:M68,1:M69</t>
+          <t>1:5G-M64,1:5G-M65,1:5G-M66,1:5G-M67,1:5G-M68,1:5G-M69</t>
         </is>
       </c>
     </row>
@@ -11160,7 +11160,7 @@
       </c>
       <c r="F359" t="inlineStr">
         <is>
-          <t>1:M64,1:M65,1:M66,1:M67,1:M68,1:M69</t>
+          <t>1:5G-M64,1:5G-M65,1:5G-M66,1:5G-M67,1:5G-M68,1:5G-M69</t>
         </is>
       </c>
     </row>
@@ -11206,7 +11206,7 @@
       </c>
       <c r="F361" t="inlineStr">
         <is>
-          <t>1:M64,1:M65,1:M66,1:M67,1:M68,1:M69</t>
+          <t>1:5G-M64,1:5G-M65,1:5G-M66,1:5G-M67,1:5G-M68,1:5G-M69</t>
         </is>
       </c>
     </row>
@@ -11257,7 +11257,7 @@
       </c>
       <c r="F363" t="inlineStr">
         <is>
-          <t>1:M64,1:M65,1:M66,1:M67,1:M68,1:M69</t>
+          <t>1:5G-M64,1:5G-M65,1:5G-M66,1:5G-M67,1:5G-M68,1:5G-M69</t>
         </is>
       </c>
     </row>
@@ -11303,7 +11303,7 @@
       </c>
       <c r="F365" t="inlineStr">
         <is>
-          <t>1:M64,1:M65,1:M66,1:M67,1:M68,1:M69</t>
+          <t>1:5G-M64,1:5G-M65,1:5G-M66,1:5G-M67,1:5G-M68,1:5G-M69</t>
         </is>
       </c>
     </row>
@@ -11355,7 +11355,7 @@
       </c>
       <c r="F367" t="inlineStr">
         <is>
-          <t>1:M64,1:M65,1:M66,1:M67,1:M68,1:M69</t>
+          <t>1:5G-M64,1:5G-M65,1:5G-M66,1:5G-M67,1:5G-M68,1:5G-M69</t>
         </is>
       </c>
     </row>
@@ -11399,7 +11399,7 @@
       </c>
       <c r="F369" t="inlineStr">
         <is>
-          <t>1:M64,1:M65,1:M66,1:M67,1:M68,1:M69</t>
+          <t>1:5G-M64,1:5G-M65,1:5G-M66,1:5G-M67,1:5G-M68,1:5G-M69</t>
         </is>
       </c>
     </row>
@@ -11443,7 +11443,7 @@
       </c>
       <c r="F371" t="inlineStr">
         <is>
-          <t>1:M64,1:M65,1:M66,1:M67,1:M68,1:M69</t>
+          <t>1:5G-M64,1:5G-M65,1:5G-M66,1:5G-M67,1:5G-M68,1:5G-M69</t>
         </is>
       </c>
     </row>
@@ -11487,7 +11487,7 @@
       </c>
       <c r="F373" t="inlineStr">
         <is>
-          <t>1:M64,1:M65,1:M66,1:M67,1:M68,1:M69</t>
+          <t>1:5G-M64,1:5G-M65,1:5G-M66,1:5G-M67,1:5G-M68,1:5G-M69</t>
         </is>
       </c>
     </row>
@@ -11531,7 +11531,7 @@
       </c>
       <c r="F375" t="inlineStr">
         <is>
-          <t>1:M64,1:M65,1:M66,1:M67,1:M68,1:M69</t>
+          <t>1:5G-M64,1:5G-M65,1:5G-M66,1:5G-M67,1:5G-M68,1:5G-M69</t>
         </is>
       </c>
     </row>
@@ -11575,7 +11575,7 @@
       </c>
       <c r="F377" t="inlineStr">
         <is>
-          <t>1:M64,1:M65,1:M66,1:M67,1:M68,1:M69</t>
+          <t>1:5G-M64,1:5G-M65,1:5G-M66,1:5G-M67,1:5G-M68,1:5G-M69</t>
         </is>
       </c>
     </row>
@@ -11619,7 +11619,7 @@
       </c>
       <c r="F379" t="inlineStr">
         <is>
-          <t>1:M64,1:M65,1:M66,1:M67,1:M68,1:M69</t>
+          <t>1:5G-M64,1:5G-M65,1:5G-M66,1:5G-M67,1:5G-M68,1:5G-M69</t>
         </is>
       </c>
     </row>
@@ -11663,7 +11663,7 @@
       </c>
       <c r="F381" t="inlineStr">
         <is>
-          <t>1:M64,1:M65,1:M66,1:M67,1:M68,1:M69</t>
+          <t>1:5G-M64,1:5G-M65,1:5G-M66,1:5G-M67,1:5G-M68,1:5G-M69</t>
         </is>
       </c>
     </row>
@@ -11707,7 +11707,7 @@
       </c>
       <c r="F383" t="inlineStr">
         <is>
-          <t>1:M64,1:M65,1:M66,1:M67,1:M68,1:M69</t>
+          <t>1:5G-M64,1:5G-M65,1:5G-M66,1:5G-M67,1:5G-M68,1:5G-M69</t>
         </is>
       </c>
     </row>
@@ -11751,7 +11751,7 @@
       </c>
       <c r="F385" t="inlineStr">
         <is>
-          <t>1:M64,1:M65,1:M66,1:M67,1:M68,1:M69</t>
+          <t>1:5G-M64,1:5G-M65,1:5G-M66,1:5G-M67,1:5G-M68,1:5G-M69</t>
         </is>
       </c>
     </row>
@@ -11795,7 +11795,7 @@
       </c>
       <c r="F387" t="inlineStr">
         <is>
-          <t>1:M64,1:M65,1:M66,1:M67,1:M68,1:M69</t>
+          <t>1:5G-M64,1:5G-M65,1:5G-M66,1:5G-M67,1:5G-M68,1:5G-M69</t>
         </is>
       </c>
     </row>
@@ -11839,7 +11839,7 @@
       </c>
       <c r="F389" t="inlineStr">
         <is>
-          <t>1:M64,1:M65,1:M66,1:M67,1:M68,1:M69</t>
+          <t>1:5G-M64,1:5G-M65,1:5G-M66,1:5G-M67,1:5G-M68,1:5G-M69</t>
         </is>
       </c>
     </row>
@@ -11883,7 +11883,7 @@
       </c>
       <c r="F391" t="inlineStr">
         <is>
-          <t>1:M64,1:M65,1:M66,1:M67,1:M68,1:M69</t>
+          <t>1:5G-M64,1:5G-M65,1:5G-M66,1:5G-M67,1:5G-M68,1:5G-M69</t>
         </is>
       </c>
     </row>
@@ -11927,7 +11927,7 @@
       </c>
       <c r="F393" t="inlineStr">
         <is>
-          <t>1:M64,1:M65,1:M66,1:M67,1:M68,1:M69</t>
+          <t>1:5G-M64,1:5G-M65,1:5G-M66,1:5G-M67,1:5G-M68,1:5G-M69</t>
         </is>
       </c>
     </row>
@@ -11971,7 +11971,7 @@
       </c>
       <c r="F395" t="inlineStr">
         <is>
-          <t>1:M64,1:M65,1:M66,1:M67,1:M68,1:M69</t>
+          <t>1:5G-M64,1:5G-M65,1:5G-M66,1:5G-M67,1:5G-M68,1:5G-M69</t>
         </is>
       </c>
     </row>
@@ -12015,7 +12015,7 @@
       </c>
       <c r="F397" t="inlineStr">
         <is>
-          <t>1:M64,1:M65,1:M66,1:M67,1:M68,1:M69</t>
+          <t>1:5G-M64,1:5G-M65,1:5G-M66,1:5G-M67,1:5G-M68,1:5G-M69</t>
         </is>
       </c>
     </row>
@@ -12059,7 +12059,7 @@
       </c>
       <c r="F399" t="inlineStr">
         <is>
-          <t>1:M64,1:M65,1:M66,1:M67,1:M68,1:M69</t>
+          <t>1:5G-M64,1:5G-M65,1:5G-M66,1:5G-M67,1:5G-M68,1:5G-M69</t>
         </is>
       </c>
     </row>
@@ -12103,7 +12103,7 @@
       </c>
       <c r="F401" t="inlineStr">
         <is>
-          <t>1:M64,1:M65,1:M66,1:M67,1:M68,1:M69</t>
+          <t>1:5G-M64,1:5G-M65,1:5G-M66,1:5G-M67,1:5G-M68,1:5G-M69</t>
         </is>
       </c>
     </row>
@@ -12147,7 +12147,7 @@
       </c>
       <c r="F403" t="inlineStr">
         <is>
-          <t>1:M64,1:M65,1:M66,1:M67,1:M68,1:M69</t>
+          <t>1:5G-M64,1:5G-M65,1:5G-M66,1:5G-M67,1:5G-M68,1:5G-M69</t>
         </is>
       </c>
     </row>
@@ -12191,7 +12191,7 @@
       </c>
       <c r="F405" t="inlineStr">
         <is>
-          <t>1:M64,1:M65,1:M66,1:M67,1:M68,1:M69</t>
+          <t>1:5G-M64,1:5G-M65,1:5G-M66,1:5G-M67,1:5G-M68,1:5G-M69</t>
         </is>
       </c>
     </row>
@@ -12235,7 +12235,7 @@
       </c>
       <c r="F407" t="inlineStr">
         <is>
-          <t>1:M64,1:M65,1:M66,1:M67,1:M68,1:M69</t>
+          <t>1:5G-M64,1:5G-M65,1:5G-M66,1:5G-M67,1:5G-M68,1:5G-M69</t>
         </is>
       </c>
     </row>
@@ -12279,7 +12279,7 @@
       </c>
       <c r="F409" t="inlineStr">
         <is>
-          <t>1:M64,1:M65,1:M66,1:M67,1:M68,1:M69</t>
+          <t>1:5G-M64,1:5G-M65,1:5G-M66,1:5G-M67,1:5G-M68,1:5G-M69</t>
         </is>
       </c>
     </row>
@@ -12323,7 +12323,7 @@
       </c>
       <c r="F411" t="inlineStr">
         <is>
-          <t>1:M64,1:M65,1:M66,1:M67,1:M68,1:M69</t>
+          <t>1:5G-M64,1:5G-M65,1:5G-M66,1:5G-M67,1:5G-M68,1:5G-M69</t>
         </is>
       </c>
     </row>
@@ -12367,7 +12367,7 @@
       </c>
       <c r="F413" t="inlineStr">
         <is>
-          <t>1:M64,1:M65,1:M66,1:M67,1:M68,1:M69</t>
+          <t>1:5G-M64,1:5G-M65,1:5G-M66,1:5G-M67,1:5G-M68,1:5G-M69</t>
         </is>
       </c>
     </row>
@@ -12411,7 +12411,7 @@
       </c>
       <c r="F415" t="inlineStr">
         <is>
-          <t>1:M64,1:M65,1:M66,1:M67,1:M68,1:M69</t>
+          <t>1:5G-M64,1:5G-M65,1:5G-M66,1:5G-M67,1:5G-M68,1:5G-M69</t>
         </is>
       </c>
     </row>
@@ -12455,7 +12455,7 @@
       </c>
       <c r="F417" t="inlineStr">
         <is>
-          <t>1:M64,1:M65,1:M66,1:M67,1:M68,1:M69</t>
+          <t>1:5G-M64,1:5G-M65,1:5G-M66,1:5G-M67,1:5G-M68,1:5G-M69</t>
         </is>
       </c>
     </row>
@@ -12499,7 +12499,7 @@
       </c>
       <c r="F419" t="inlineStr">
         <is>
-          <t>1:M64,1:M65,1:M66,1:M67,1:M68,1:M69</t>
+          <t>1:5G-M64,1:5G-M65,1:5G-M66,1:5G-M67,1:5G-M68,1:5G-M69</t>
         </is>
       </c>
     </row>
@@ -12543,7 +12543,7 @@
       </c>
       <c r="F421" t="inlineStr">
         <is>
-          <t>1:M64,1:M65,1:M66,1:M67,1:M68,1:M69</t>
+          <t>1:5G-M64,1:5G-M65,1:5G-M66,1:5G-M67,1:5G-M68,1:5G-M69</t>
         </is>
       </c>
     </row>
@@ -12587,7 +12587,7 @@
       </c>
       <c r="F423" t="inlineStr">
         <is>
-          <t>1:M64,1:M65,1:M66,1:M67,1:M68,1:M69</t>
+          <t>1:5G-M64,1:5G-M65,1:5G-M66,1:5G-M67,1:5G-M68,1:5G-M69</t>
         </is>
       </c>
     </row>
@@ -12631,7 +12631,7 @@
       </c>
       <c r="F425" t="inlineStr">
         <is>
-          <t>1:M64,1:M65,1:M66,1:M67,1:M68,1:M69</t>
+          <t>1:5G-M64,1:5G-M65,1:5G-M66,1:5G-M67,1:5G-M68,1:5G-M69</t>
         </is>
       </c>
     </row>
@@ -12675,7 +12675,7 @@
       </c>
       <c r="F427" t="inlineStr">
         <is>
-          <t>1:M64,1:M65,1:M66,1:M67,1:M68,1:M69</t>
+          <t>1:5G-M64,1:5G-M65,1:5G-M66,1:5G-M67,1:5G-M68,1:5G-M69</t>
         </is>
       </c>
     </row>
@@ -12719,7 +12719,7 @@
       </c>
       <c r="F429" t="inlineStr">
         <is>
-          <t>1:M64,1:M65,1:M66,1:M67,1:M68,1:M69</t>
+          <t>1:5G-M64,1:5G-M65,1:5G-M66,1:5G-M67,1:5G-M68,1:5G-M69</t>
         </is>
       </c>
     </row>
@@ -12763,7 +12763,7 @@
       </c>
       <c r="F431" t="inlineStr">
         <is>
-          <t>1:M64,1:M65,1:M66,1:M67,1:M68,1:M69</t>
+          <t>1:5G-M64,1:5G-M65,1:5G-M66,1:5G-M67,1:5G-M68,1:5G-M69</t>
         </is>
       </c>
     </row>
@@ -12811,7 +12811,7 @@
       </c>
       <c r="F433" t="inlineStr">
         <is>
-          <t>1:M64,1:M65,1:M66,1:M67,1:M68,1:M69</t>
+          <t>1:5G-M64,1:5G-M65,1:5G-M66,1:5G-M67,1:5G-M68,1:5G-M69</t>
         </is>
       </c>
     </row>
@@ -12865,7 +12865,7 @@
       </c>
       <c r="F435" t="inlineStr">
         <is>
-          <t>1:M64,1:M65,1:M66,1:M67,1:M68,1:M69</t>
+          <t>1:5G-M64,1:5G-M65,1:5G-M66,1:5G-M67,1:5G-M68,1:5G-M69</t>
         </is>
       </c>
     </row>
@@ -12916,7 +12916,7 @@
       </c>
       <c r="F437" t="inlineStr">
         <is>
-          <t>1:M64,1:M65,1:M66,1:M67,1:M68,1:M69</t>
+          <t>1:5G-M64,1:5G-M65,1:5G-M66,1:5G-M67,1:5G-M68,1:5G-M69</t>
         </is>
       </c>
     </row>
@@ -12962,7 +12962,7 @@
       </c>
       <c r="F439" t="inlineStr">
         <is>
-          <t>1:M64,1:M65,1:M66,1:M67,1:M68,1:M69</t>
+          <t>1:5G-M64,1:5G-M65,1:5G-M66,1:5G-M67,1:5G-M68,1:5G-M69</t>
         </is>
       </c>
     </row>
@@ -13010,7 +13010,7 @@
       </c>
       <c r="F441" t="inlineStr">
         <is>
-          <t>1:M64,1:M65,1:M66,1:M67,1:M68,1:M69</t>
+          <t>1:5G-M64,1:5G-M65,1:5G-M66,1:5G-M67,1:5G-M68,1:5G-M69</t>
         </is>
       </c>
     </row>
@@ -13065,7 +13065,7 @@
       </c>
       <c r="F443" t="inlineStr">
         <is>
-          <t>1:M64,1:M65,1:M66,1:M67,1:M68,1:M69</t>
+          <t>1:5G-M64,1:5G-M65,1:5G-M66,1:5G-M67,1:5G-M68,1:5G-M69</t>
         </is>
       </c>
     </row>
@@ -13111,7 +13111,7 @@
       </c>
       <c r="F445" t="inlineStr">
         <is>
-          <t>1:M64,1:M65,1:M66,1:M67,1:M68,1:M69</t>
+          <t>1:5G-M64,1:5G-M65,1:5G-M66,1:5G-M67,1:5G-M68,1:5G-M69</t>
         </is>
       </c>
     </row>
@@ -13162,7 +13162,7 @@
       </c>
       <c r="F447" t="inlineStr">
         <is>
-          <t>1:M64,1:M65,1:M66,1:M67,1:M68,1:M69</t>
+          <t>1:5G-M64,1:5G-M65,1:5G-M66,1:5G-M67,1:5G-M68,1:5G-M69</t>
         </is>
       </c>
     </row>
@@ -13217,7 +13217,7 @@
       </c>
       <c r="F449" t="inlineStr">
         <is>
-          <t>1:M64,1:M65,1:M66,1:M67,1:M68,1:M69</t>
+          <t>1:5G-M64,1:5G-M65,1:5G-M66,1:5G-M67,1:5G-M68,1:5G-M69</t>
         </is>
       </c>
     </row>
@@ -13265,7 +13265,7 @@
       </c>
       <c r="F451" t="inlineStr">
         <is>
-          <t>1:M64,1:M65,1:M66,1:M67,1:M68,1:M69</t>
+          <t>1:5G-M64,1:5G-M65,1:5G-M66,1:5G-M67,1:5G-M68,1:5G-M69</t>
         </is>
       </c>
     </row>
@@ -13309,7 +13309,7 @@
       </c>
       <c r="F453" t="inlineStr">
         <is>
-          <t>1:M64,1:M65,1:M66,1:M67,1:M68,1:M69</t>
+          <t>1:5G-M64,1:5G-M65,1:5G-M66,1:5G-M67,1:5G-M68,1:5G-M69</t>
         </is>
       </c>
     </row>
@@ -13353,7 +13353,7 @@
       </c>
       <c r="F455" t="inlineStr">
         <is>
-          <t>1:M64,1:M65,1:M66,1:M67,1:M68,1:M69</t>
+          <t>1:5G-M64,1:5G-M65,1:5G-M66,1:5G-M67,1:5G-M68,1:5G-M69</t>
         </is>
       </c>
     </row>
@@ -13398,7 +13398,7 @@
       </c>
       <c r="F457" t="inlineStr">
         <is>
-          <t>1:M64,1:M65,1:M66,1:M67,1:M68,1:M69</t>
+          <t>1:5G-M64,1:5G-M65,1:5G-M66,1:5G-M67,1:5G-M68,1:5G-M69</t>
         </is>
       </c>
     </row>
@@ -13442,7 +13442,7 @@
       </c>
       <c r="F459" t="inlineStr">
         <is>
-          <t>1:M64,1:M65,1:M66,1:M67,1:M68,1:M69</t>
+          <t>1:5G-M64,1:5G-M65,1:5G-M66,1:5G-M67,1:5G-M68,1:5G-M69</t>
         </is>
       </c>
     </row>
@@ -13489,7 +13489,7 @@
       </c>
       <c r="F461" t="inlineStr">
         <is>
-          <t>1:M64,1:M65,1:M66,1:M67,1:M68,1:M69</t>
+          <t>1:5G-M64,1:5G-M65,1:5G-M66,1:5G-M67,1:5G-M68,1:5G-M69</t>
         </is>
       </c>
     </row>
@@ -13533,7 +13533,7 @@
       </c>
       <c r="F463" t="inlineStr">
         <is>
-          <t>1:M64,1:M65,1:M66,1:M67,1:M68,1:M69</t>
+          <t>1:5G-M64,1:5G-M65,1:5G-M66,1:5G-M67,1:5G-M68,1:5G-M69</t>
         </is>
       </c>
     </row>
@@ -13577,7 +13577,7 @@
       </c>
       <c r="F465" t="inlineStr">
         <is>
-          <t>1:M64,1:M65,1:M66,1:M67,1:M68,1:M69</t>
+          <t>1:5G-M64,1:5G-M65,1:5G-M66,1:5G-M67,1:5G-M68,1:5G-M69</t>
         </is>
       </c>
     </row>
@@ -13622,7 +13622,7 @@
       </c>
       <c r="F467" t="inlineStr">
         <is>
-          <t>1:M64,1:M65,1:M66,1:M67,1:M68,1:M69</t>
+          <t>1:5G-M64,1:5G-M65,1:5G-M66,1:5G-M67,1:5G-M68,1:5G-M69</t>
         </is>
       </c>
     </row>
@@ -13667,7 +13667,7 @@
       </c>
       <c r="F469" t="inlineStr">
         <is>
-          <t>1:M64,1:M65,1:M66,1:M67,1:M68,1:M69</t>
+          <t>1:5G-M64,1:5G-M65,1:5G-M66,1:5G-M67,1:5G-M68,1:5G-M69</t>
         </is>
       </c>
     </row>
@@ -13711,7 +13711,7 @@
       </c>
       <c r="F471" t="inlineStr">
         <is>
-          <t>1:M64,1:M65,1:M66,1:M67,1:M68,1:M69</t>
+          <t>1:5G-M64,1:5G-M65,1:5G-M66,1:5G-M67,1:5G-M68,1:5G-M69</t>
         </is>
       </c>
     </row>
@@ -13755,7 +13755,7 @@
       </c>
       <c r="F473" t="inlineStr">
         <is>
-          <t>1:M64,1:M65,1:M66,1:M67,1:M68,1:M69</t>
+          <t>1:5G-M64,1:5G-M65,1:5G-M66,1:5G-M67,1:5G-M68,1:5G-M69</t>
         </is>
       </c>
     </row>
@@ -13799,7 +13799,7 @@
       </c>
       <c r="F475" t="inlineStr">
         <is>
-          <t>1:M64,1:M65,1:M66,1:M67,1:M68,1:M69</t>
+          <t>1:5G-M64,1:5G-M65,1:5G-M66,1:5G-M67,1:5G-M68,1:5G-M69</t>
         </is>
       </c>
     </row>
@@ -13843,7 +13843,7 @@
       </c>
       <c r="F477" t="inlineStr">
         <is>
-          <t>1:M64,1:M65,1:M66,1:M67,1:M68,1:M69</t>
+          <t>1:5G-M64,1:5G-M65,1:5G-M66,1:5G-M67,1:5G-M68,1:5G-M69</t>
         </is>
       </c>
     </row>
@@ -13887,7 +13887,7 @@
       </c>
       <c r="F479" t="inlineStr">
         <is>
-          <t>1:M64,1:M65,1:M66,1:M67,1:M68,1:M69</t>
+          <t>1:5G-M64,1:5G-M65,1:5G-M66,1:5G-M67,1:5G-M68,1:5G-M69</t>
         </is>
       </c>
     </row>
@@ -13931,7 +13931,7 @@
       </c>
       <c r="F481" t="inlineStr">
         <is>
-          <t>1:M64,1:M65,1:M66,1:M67,1:M68,1:M69</t>
+          <t>1:5G-M64,1:5G-M65,1:5G-M66,1:5G-M67,1:5G-M68,1:5G-M69</t>
         </is>
       </c>
     </row>
@@ -13975,7 +13975,7 @@
       </c>
       <c r="F483" t="inlineStr">
         <is>
-          <t>1:M64,1:M65,1:M66,1:M67,1:M68,1:M69</t>
+          <t>1:5G-M64,1:5G-M65,1:5G-M66,1:5G-M67,1:5G-M68,1:5G-M69</t>
         </is>
       </c>
     </row>
@@ -14021,7 +14021,7 @@
       </c>
       <c r="F485" t="inlineStr">
         <is>
-          <t>1:M64,1:M65,1:M66,1:M67,1:M68,1:M69</t>
+          <t>1:5G-M64,1:5G-M65,1:5G-M66,1:5G-M67,1:5G-M68,1:5G-M69</t>
         </is>
       </c>
     </row>
@@ -14069,7 +14069,7 @@
       </c>
       <c r="F487" t="inlineStr">
         <is>
-          <t>1:M64,1:M65,1:M66,1:M67,1:M68,1:M69</t>
+          <t>1:5G-M64,1:5G-M65,1:5G-M66,1:5G-M67,1:5G-M68,1:5G-M69</t>
         </is>
       </c>
     </row>
@@ -14120,7 +14120,7 @@
       </c>
       <c r="F489" t="inlineStr">
         <is>
-          <t>1:M64,1:M65,1:M66,1:M67,1:M68,1:M69</t>
+          <t>1:5G-M64,1:5G-M65,1:5G-M66,1:5G-M67,1:5G-M68,1:5G-M69</t>
         </is>
       </c>
     </row>
@@ -14164,7 +14164,7 @@
       </c>
       <c r="F491" t="inlineStr">
         <is>
-          <t>1:M64,1:M65,1:M66,1:M67,1:M68,1:M69</t>
+          <t>1:5G-M64,1:5G-M65,1:5G-M66,1:5G-M67,1:5G-M68,1:5G-M69</t>
         </is>
       </c>
     </row>
@@ -14208,7 +14208,7 @@
       </c>
       <c r="F493" t="inlineStr">
         <is>
-          <t>1:M64,1:M65,1:M66,1:M67,1:M68,1:M69</t>
+          <t>1:5G-M64,1:5G-M65,1:5G-M66,1:5G-M67,1:5G-M68,1:5G-M69</t>
         </is>
       </c>
     </row>
@@ -14252,7 +14252,7 @@
       </c>
       <c r="F495" t="inlineStr">
         <is>
-          <t>1:M64,1:M65,1:M66,1:M67,1:M68,1:M69</t>
+          <t>1:5G-M64,1:5G-M65,1:5G-M66,1:5G-M67,1:5G-M68,1:5G-M69</t>
         </is>
       </c>
     </row>
@@ -14296,7 +14296,7 @@
       </c>
       <c r="F497" t="inlineStr">
         <is>
-          <t>1:M64,1:M65,1:M66,1:M67,1:M68,1:M69</t>
+          <t>1:5G-M64,1:5G-M65,1:5G-M66,1:5G-M67,1:5G-M68,1:5G-M69</t>
         </is>
       </c>
     </row>
@@ -14347,7 +14347,7 @@
       </c>
       <c r="F499" t="inlineStr">
         <is>
-          <t>1:M64,1:M65,1:M66,1:M67,1:M68,1:M69</t>
+          <t>1:5G-M64,1:5G-M65,1:5G-M66,1:5G-M67,1:5G-M68,1:5G-M69</t>
         </is>
       </c>
     </row>
@@ -14393,7 +14393,7 @@
       </c>
       <c r="F501" t="inlineStr">
         <is>
-          <t>1:M64,1:M65,1:M66,1:M67,1:M68,1:M69</t>
+          <t>1:5G-M64,1:5G-M65,1:5G-M66,1:5G-M67,1:5G-M68,1:5G-M69</t>
         </is>
       </c>
     </row>
@@ -14461,7 +14461,7 @@
       </c>
       <c r="F504" t="inlineStr">
         <is>
-          <t>1:M70,1:M71,1:M72,1:M73,1:M74</t>
+          <t>1:5G-M70,1:5G-M71,1:5G-M72,1:5G-M73,1:5G-M74</t>
         </is>
       </c>
     </row>
@@ -14505,7 +14505,7 @@
       </c>
       <c r="F506" t="inlineStr">
         <is>
-          <t>1:M70,1:M71,1:M72,1:M73,1:M74</t>
+          <t>1:5G-M70,1:5G-M71,1:5G-M72,1:5G-M73,1:5G-M74</t>
         </is>
       </c>
     </row>
@@ -14549,7 +14549,7 @@
       </c>
       <c r="F508" t="inlineStr">
         <is>
-          <t>1:M70,1:M71,1:M72,1:M73,1:M74</t>
+          <t>1:5G-M70,1:5G-M71,1:5G-M72,1:5G-M73,1:5G-M74</t>
         </is>
       </c>
     </row>
@@ -14593,7 +14593,7 @@
       </c>
       <c r="F510" t="inlineStr">
         <is>
-          <t>1:M70,1:M71,1:M72,1:M73,1:M74</t>
+          <t>1:5G-M70,1:5G-M71,1:5G-M72,1:5G-M73,1:5G-M74</t>
         </is>
       </c>
     </row>
@@ -14637,7 +14637,7 @@
       </c>
       <c r="F512" t="inlineStr">
         <is>
-          <t>1:M70,1:M71,1:M72,1:M73,1:M74</t>
+          <t>1:5G-M70,1:5G-M71,1:5G-M72,1:5G-M73,1:5G-M74</t>
         </is>
       </c>
     </row>
@@ -14681,7 +14681,7 @@
       </c>
       <c r="F514" t="inlineStr">
         <is>
-          <t>1:M70,1:M71,1:M72,1:M73,1:M74</t>
+          <t>1:5G-M70,1:5G-M71,1:5G-M72,1:5G-M73,1:5G-M74</t>
         </is>
       </c>
     </row>
@@ -14725,7 +14725,7 @@
       </c>
       <c r="F516" t="inlineStr">
         <is>
-          <t>1:M70,1:M71,1:M72,1:M73,1:M74</t>
+          <t>1:5G-M70,1:5G-M71,1:5G-M72,1:5G-M73,1:5G-M74</t>
         </is>
       </c>
     </row>
@@ -14769,7 +14769,7 @@
       </c>
       <c r="F518" t="inlineStr">
         <is>
-          <t>1:M70,1:M71,1:M72,1:M73,1:M74</t>
+          <t>1:5G-M70,1:5G-M71,1:5G-M72,1:5G-M73,1:5G-M74</t>
         </is>
       </c>
     </row>
@@ -14813,7 +14813,7 @@
       </c>
       <c r="F520" t="inlineStr">
         <is>
-          <t>1:M70,1:M71,1:M72,1:M73,1:M74</t>
+          <t>1:5G-M70,1:5G-M71,1:5G-M72,1:5G-M73,1:5G-M74</t>
         </is>
       </c>
     </row>
@@ -14858,7 +14858,7 @@
       </c>
       <c r="F522" t="inlineStr">
         <is>
-          <t>1:M70,1:M71,1:M72,1:M73,1:M74</t>
+          <t>1:5G-M70,1:5G-M71,1:5G-M72,1:5G-M73,1:5G-M74</t>
         </is>
       </c>
     </row>
@@ -14905,7 +14905,7 @@
       </c>
       <c r="F524" t="inlineStr">
         <is>
-          <t>1:M70,1:M71,1:M72,1:M73,1:M74</t>
+          <t>1:5G-M70,1:5G-M71,1:5G-M72,1:5G-M73,1:5G-M74</t>
         </is>
       </c>
     </row>
@@ -14950,7 +14950,7 @@
       </c>
       <c r="F526" t="inlineStr">
         <is>
-          <t>1:M70,1:M71,1:M72,1:M73,1:M74</t>
+          <t>1:5G-M70,1:5G-M71,1:5G-M72,1:5G-M73,1:5G-M74</t>
         </is>
       </c>
     </row>
@@ -14994,7 +14994,7 @@
       </c>
       <c r="F528" t="inlineStr">
         <is>
-          <t>1:M70,1:M71,1:M72,1:M73,1:M74</t>
+          <t>1:5G-M70,1:5G-M71,1:5G-M72,1:5G-M73,1:5G-M74</t>
         </is>
       </c>
     </row>
@@ -15038,7 +15038,7 @@
       </c>
       <c r="F530" t="inlineStr">
         <is>
-          <t>1:M70,1:M71,1:M72,1:M73,1:M74</t>
+          <t>1:5G-M70,1:5G-M71,1:5G-M72,1:5G-M73,1:5G-M74</t>
         </is>
       </c>
     </row>
@@ -15082,7 +15082,7 @@
       </c>
       <c r="F532" t="inlineStr">
         <is>
-          <t>1:M70,1:M71,1:M72,1:M73,1:M74</t>
+          <t>1:5G-M70,1:5G-M71,1:5G-M72,1:5G-M73,1:5G-M74</t>
         </is>
       </c>
     </row>
@@ -15126,7 +15126,7 @@
       </c>
       <c r="F534" t="inlineStr">
         <is>
-          <t>1:M70,1:M71,1:M72,1:M73,1:M74</t>
+          <t>1:5G-M70,1:5G-M71,1:5G-M72,1:5G-M73,1:5G-M74</t>
         </is>
       </c>
     </row>
@@ -15170,7 +15170,7 @@
       </c>
       <c r="F536" t="inlineStr">
         <is>
-          <t>1:M70,1:M71,1:M72,1:M73,1:M74</t>
+          <t>1:5G-M70,1:5G-M71,1:5G-M72,1:5G-M73,1:5G-M74</t>
         </is>
       </c>
     </row>
@@ -15214,7 +15214,7 @@
       </c>
       <c r="F538" t="inlineStr">
         <is>
-          <t>1:M70,1:M71,1:M72,1:M73,1:M74</t>
+          <t>1:5G-M70,1:5G-M71,1:5G-M72,1:5G-M73,1:5G-M74</t>
         </is>
       </c>
     </row>
@@ -15258,7 +15258,7 @@
       </c>
       <c r="F540" t="inlineStr">
         <is>
-          <t>1:M70,1:M71,1:M72,1:M73,1:M74</t>
+          <t>1:5G-M70,1:5G-M71,1:5G-M72,1:5G-M73,1:5G-M74</t>
         </is>
       </c>
     </row>
@@ -15302,7 +15302,7 @@
       </c>
       <c r="F542" t="inlineStr">
         <is>
-          <t>1:M70,1:M71,1:M72,1:M73,1:M74</t>
+          <t>1:5G-M70,1:5G-M71,1:5G-M72,1:5G-M73,1:5G-M74</t>
         </is>
       </c>
     </row>
@@ -15346,7 +15346,7 @@
       </c>
       <c r="F544" t="inlineStr">
         <is>
-          <t>1:M70,1:M71,1:M72,1:M73,1:M74</t>
+          <t>1:5G-M70,1:5G-M71,1:5G-M72,1:5G-M73,1:5G-M74</t>
         </is>
       </c>
     </row>
@@ -15390,7 +15390,7 @@
       </c>
       <c r="F546" t="inlineStr">
         <is>
-          <t>1:M70,1:M71,1:M72,1:M73,1:M74</t>
+          <t>1:5G-M70,1:5G-M71,1:5G-M72,1:5G-M73,1:5G-M74</t>
         </is>
       </c>
     </row>
@@ -15434,7 +15434,7 @@
       </c>
       <c r="F548" t="inlineStr">
         <is>
-          <t>1:M70,1:M71,1:M72,1:M73,1:M74</t>
+          <t>1:5G-M70,1:5G-M71,1:5G-M72,1:5G-M73,1:5G-M74</t>
         </is>
       </c>
     </row>
@@ -15478,7 +15478,7 @@
       </c>
       <c r="F550" t="inlineStr">
         <is>
-          <t>1:M70,1:M71,1:M72,1:M73,1:M74</t>
+          <t>1:5G-M70,1:5G-M71,1:5G-M72,1:5G-M73,1:5G-M74</t>
         </is>
       </c>
     </row>
@@ -15522,7 +15522,7 @@
       </c>
       <c r="F552" t="inlineStr">
         <is>
-          <t>1:M70,1:M71,1:M72,1:M73,1:M74</t>
+          <t>1:5G-M70,1:5G-M71,1:5G-M72,1:5G-M73,1:5G-M74</t>
         </is>
       </c>
     </row>
@@ -15566,7 +15566,7 @@
       </c>
       <c r="F554" t="inlineStr">
         <is>
-          <t>1:M70,1:M71,1:M72,1:M73,1:M74</t>
+          <t>1:5G-M70,1:5G-M71,1:5G-M72,1:5G-M73,1:5G-M74</t>
         </is>
       </c>
     </row>
@@ -15610,7 +15610,7 @@
       </c>
       <c r="F556" t="inlineStr">
         <is>
-          <t>1:M70,1:M71,1:M72,1:M73,1:M74</t>
+          <t>1:5G-M70,1:5G-M71,1:5G-M72,1:5G-M73,1:5G-M74</t>
         </is>
       </c>
     </row>
@@ -15654,7 +15654,7 @@
       </c>
       <c r="F558" t="inlineStr">
         <is>
-          <t>1:M70,1:M71,1:M72,1:M73,1:M74</t>
+          <t>1:5G-M70,1:5G-M71,1:5G-M72,1:5G-M73,1:5G-M74</t>
         </is>
       </c>
     </row>
@@ -15698,7 +15698,7 @@
       </c>
       <c r="F560" t="inlineStr">
         <is>
-          <t>1:M70,1:M71,1:M72,1:M73,1:M74</t>
+          <t>1:5G-M70,1:5G-M71,1:5G-M72,1:5G-M73,1:5G-M74</t>
         </is>
       </c>
     </row>
@@ -15742,7 +15742,7 @@
       </c>
       <c r="F562" t="inlineStr">
         <is>
-          <t>1:M70,1:M71,1:M72,1:M73,1:M74</t>
+          <t>1:5G-M70,1:5G-M71,1:5G-M72,1:5G-M73,1:5G-M74</t>
         </is>
       </c>
     </row>
@@ -15786,7 +15786,7 @@
       </c>
       <c r="F564" t="inlineStr">
         <is>
-          <t>1:M70,1:M71,1:M72,1:M73,1:M74</t>
+          <t>1:5G-M70,1:5G-M71,1:5G-M72,1:5G-M73,1:5G-M74</t>
         </is>
       </c>
     </row>
@@ -15830,7 +15830,7 @@
       </c>
       <c r="F566" t="inlineStr">
         <is>
-          <t>1:M70,1:M71,1:M72,1:M73,1:M74</t>
+          <t>1:5G-M70,1:5G-M71,1:5G-M72,1:5G-M73,1:5G-M74</t>
         </is>
       </c>
     </row>
@@ -15874,7 +15874,7 @@
       </c>
       <c r="F568" t="inlineStr">
         <is>
-          <t>1:M70,1:M71,1:M72,1:M73,1:M74</t>
+          <t>1:5G-M70,1:5G-M71,1:5G-M72,1:5G-M73,1:5G-M74</t>
         </is>
       </c>
     </row>
@@ -15918,7 +15918,7 @@
       </c>
       <c r="F570" t="inlineStr">
         <is>
-          <t>1:M70,1:M71,1:M72,1:M73,1:M74</t>
+          <t>1:5G-M70,1:5G-M71,1:5G-M72,1:5G-M73,1:5G-M74</t>
         </is>
       </c>
     </row>
@@ -15962,7 +15962,7 @@
       </c>
       <c r="F572" t="inlineStr">
         <is>
-          <t>1:M70,1:M71,1:M72,1:M73,1:M74</t>
+          <t>1:5G-M70,1:5G-M71,1:5G-M72,1:5G-M73,1:5G-M74</t>
         </is>
       </c>
     </row>
@@ -16006,7 +16006,7 @@
       </c>
       <c r="F574" t="inlineStr">
         <is>
-          <t>1:M70,1:M71,1:M72,1:M73,1:M74</t>
+          <t>1:5G-M70,1:5G-M71,1:5G-M72,1:5G-M73,1:5G-M74</t>
         </is>
       </c>
     </row>
@@ -16050,7 +16050,7 @@
       </c>
       <c r="F576" t="inlineStr">
         <is>
-          <t>1:M70,1:M71,1:M72,1:M73,1:M74</t>
+          <t>1:5G-M70,1:5G-M71,1:5G-M72,1:5G-M73,1:5G-M74</t>
         </is>
       </c>
     </row>
@@ -16116,7 +16116,7 @@
       </c>
       <c r="F579" t="inlineStr">
         <is>
-          <t>1:M75,1:M76,1:M77,1:M78,1:M79</t>
+          <t>1:5G-M75,1:5G-M76,1:5G-M77,1:5G-M78,1:5G-M79</t>
         </is>
       </c>
     </row>
@@ -16160,7 +16160,7 @@
       </c>
       <c r="F581" t="inlineStr">
         <is>
-          <t>1:M75,1:M76,1:M77,1:M78,1:M79</t>
+          <t>1:5G-M75,1:5G-M76,1:5G-M77,1:5G-M78,1:5G-M79</t>
         </is>
       </c>
     </row>
@@ -16204,7 +16204,7 @@
       </c>
       <c r="F583" t="inlineStr">
         <is>
-          <t>1:M75,1:M76,1:M77,1:M78,1:M79</t>
+          <t>1:5G-M75,1:5G-M76,1:5G-M77,1:5G-M78,1:5G-M79</t>
         </is>
       </c>
     </row>
@@ -16248,7 +16248,7 @@
       </c>
       <c r="F585" t="inlineStr">
         <is>
-          <t>1:M75,1:M76,1:M77,1:M78,1:M79</t>
+          <t>1:5G-M75,1:5G-M76,1:5G-M77,1:5G-M78,1:5G-M79</t>
         </is>
       </c>
     </row>
@@ -16292,7 +16292,7 @@
       </c>
       <c r="F587" t="inlineStr">
         <is>
-          <t>1:M75,1:M76,1:M77,1:M78,1:M79</t>
+          <t>1:5G-M75,1:5G-M76,1:5G-M77,1:5G-M78,1:5G-M79</t>
         </is>
       </c>
     </row>
@@ -16336,7 +16336,7 @@
       </c>
       <c r="F589" t="inlineStr">
         <is>
-          <t>1:M75,1:M76,1:M77,1:M78,1:M79</t>
+          <t>1:5G-M75,1:5G-M76,1:5G-M77,1:5G-M78,1:5G-M79</t>
         </is>
       </c>
     </row>
@@ -16380,7 +16380,7 @@
       </c>
       <c r="F591" t="inlineStr">
         <is>
-          <t>1:M75,1:M76,1:M77,1:M78,1:M79</t>
+          <t>1:5G-M75,1:5G-M76,1:5G-M77,1:5G-M78,1:5G-M79</t>
         </is>
       </c>
     </row>
@@ -16424,7 +16424,7 @@
       </c>
       <c r="F593" t="inlineStr">
         <is>
-          <t>1:M75,1:M76,1:M77,1:M78,1:M79</t>
+          <t>1:5G-M75,1:5G-M76,1:5G-M77,1:5G-M78,1:5G-M79</t>
         </is>
       </c>
     </row>
@@ -16468,7 +16468,7 @@
       </c>
       <c r="F595" t="inlineStr">
         <is>
-          <t>1:M75,1:M76,1:M77,1:M78,1:M79</t>
+          <t>1:5G-M75,1:5G-M76,1:5G-M77,1:5G-M78,1:5G-M79</t>
         </is>
       </c>
     </row>
@@ -16512,7 +16512,7 @@
       </c>
       <c r="F597" t="inlineStr">
         <is>
-          <t>1:M75,1:M76,1:M77,1:M78,1:M79</t>
+          <t>1:5G-M75,1:5G-M76,1:5G-M77,1:5G-M78,1:5G-M79</t>
         </is>
       </c>
     </row>
@@ -16556,7 +16556,7 @@
       </c>
       <c r="F599" t="inlineStr">
         <is>
-          <t>1:M75,1:M76,1:M77,1:M78,1:M79</t>
+          <t>1:5G-M75,1:5G-M76,1:5G-M77,1:5G-M78,1:5G-M79</t>
         </is>
       </c>
     </row>
@@ -16608,7 +16608,7 @@
       </c>
       <c r="F601" t="inlineStr">
         <is>
-          <t>1:M75,1:M76,1:M77,1:M78,1:M79</t>
+          <t>1:5G-M75,1:5G-M76,1:5G-M77,1:5G-M78,1:5G-M79</t>
         </is>
       </c>
     </row>
@@ -16657,7 +16657,7 @@
       </c>
       <c r="F603" t="inlineStr">
         <is>
-          <t>1:M75,1:M76,1:M77,1:M78,1:M79</t>
+          <t>1:5G-M75,1:5G-M76,1:5G-M77,1:5G-M78,1:5G-M79</t>
         </is>
       </c>
     </row>
@@ -16706,7 +16706,7 @@
       </c>
       <c r="F605" t="inlineStr">
         <is>
-          <t>1:M75,1:M76,1:M77,1:M78,1:M79</t>
+          <t>1:5G-M75,1:5G-M76,1:5G-M77,1:5G-M78,1:5G-M79</t>
         </is>
       </c>
     </row>
@@ -16751,7 +16751,7 @@
       </c>
       <c r="F607" t="inlineStr">
         <is>
-          <t>1:M75,1:M76,1:M77,1:M78,1:M79</t>
+          <t>1:5G-M75,1:5G-M76,1:5G-M77,1:5G-M78,1:5G-M79</t>
         </is>
       </c>
     </row>
@@ -16839,7 +16839,7 @@
       </c>
       <c r="F611" t="inlineStr">
         <is>
-          <t>1:M80,1:M81,1:M82</t>
+          <t>1:5G-M80,1:5G-M81,1:5G-M82</t>
         </is>
       </c>
     </row>
@@ -16883,7 +16883,7 @@
       </c>
       <c r="F613" t="inlineStr">
         <is>
-          <t>1:M80,1:M81,1:M82</t>
+          <t>1:5G-M80,1:5G-M81,1:5G-M82</t>
         </is>
       </c>
     </row>
@@ -16927,7 +16927,7 @@
       </c>
       <c r="F615" t="inlineStr">
         <is>
-          <t>1:M80,1:M81,1:M82</t>
+          <t>1:5G-M80,1:5G-M81,1:5G-M82</t>
         </is>
       </c>
     </row>
@@ -16971,7 +16971,7 @@
       </c>
       <c r="F617" t="inlineStr">
         <is>
-          <t>1:M80,1:M81,1:M82</t>
+          <t>1:5G-M80,1:5G-M81,1:5G-M82</t>
         </is>
       </c>
     </row>
@@ -17015,7 +17015,7 @@
       </c>
       <c r="F619" t="inlineStr">
         <is>
-          <t>1:M80,1:M81,1:M82</t>
+          <t>1:5G-M80,1:5G-M81,1:5G-M82</t>
         </is>
       </c>
     </row>
@@ -17059,7 +17059,7 @@
       </c>
       <c r="F621" t="inlineStr">
         <is>
-          <t>1:M80,1:M81,1:M82</t>
+          <t>1:5G-M80,1:5G-M81,1:5G-M82</t>
         </is>
       </c>
     </row>
@@ -17103,7 +17103,7 @@
       </c>
       <c r="F623" t="inlineStr">
         <is>
-          <t>1:M80,1:M81,1:M82</t>
+          <t>1:5G-M80,1:5G-M81,1:5G-M82</t>
         </is>
       </c>
     </row>
@@ -17147,7 +17147,7 @@
       </c>
       <c r="F625" t="inlineStr">
         <is>
-          <t>1:M80,1:M81,1:M82</t>
+          <t>1:5G-M80,1:5G-M81,1:5G-M82</t>
         </is>
       </c>
     </row>
@@ -17191,7 +17191,7 @@
       </c>
       <c r="F627" t="inlineStr">
         <is>
-          <t>1:M80,1:M81,1:M82</t>
+          <t>1:5G-M80,1:5G-M81,1:5G-M82</t>
         </is>
       </c>
     </row>
@@ -17235,7 +17235,7 @@
       </c>
       <c r="F629" t="inlineStr">
         <is>
-          <t>1:M80,1:M81,1:M82</t>
+          <t>1:5G-M80,1:5G-M81,1:5G-M82</t>
         </is>
       </c>
     </row>
@@ -17279,7 +17279,7 @@
       </c>
       <c r="F631" t="inlineStr">
         <is>
-          <t>1:M80,1:M81,1:M82</t>
+          <t>1:5G-M80,1:5G-M81,1:5G-M82</t>
         </is>
       </c>
     </row>
@@ -17323,7 +17323,7 @@
       </c>
       <c r="F633" t="inlineStr">
         <is>
-          <t>1:M80,1:M81,1:M82</t>
+          <t>1:5G-M80,1:5G-M81,1:5G-M82</t>
         </is>
       </c>
     </row>
@@ -17367,7 +17367,7 @@
       </c>
       <c r="F635" t="inlineStr">
         <is>
-          <t>1:M80,1:M81,1:M82</t>
+          <t>1:5G-M80,1:5G-M81,1:5G-M82</t>
         </is>
       </c>
     </row>
@@ -17411,7 +17411,7 @@
       </c>
       <c r="F637" t="inlineStr">
         <is>
-          <t>1:M80,1:M81,1:M82</t>
+          <t>1:5G-M80,1:5G-M81,1:5G-M82</t>
         </is>
       </c>
     </row>
@@ -17455,7 +17455,7 @@
       </c>
       <c r="F639" t="inlineStr">
         <is>
-          <t>1:M80,1:M81,1:M82</t>
+          <t>1:5G-M80,1:5G-M81,1:5G-M82</t>
         </is>
       </c>
     </row>
@@ -17499,7 +17499,7 @@
       </c>
       <c r="F641" t="inlineStr">
         <is>
-          <t>1:M80,1:M81,1:M82</t>
+          <t>1:5G-M80,1:5G-M81,1:5G-M82</t>
         </is>
       </c>
     </row>
@@ -17543,7 +17543,7 @@
       </c>
       <c r="F643" t="inlineStr">
         <is>
-          <t>1:M80,1:M81,1:M82</t>
+          <t>1:5G-M80,1:5G-M81,1:5G-M82</t>
         </is>
       </c>
     </row>
@@ -17587,7 +17587,7 @@
       </c>
       <c r="F645" t="inlineStr">
         <is>
-          <t>1:M80,1:M81,1:M82</t>
+          <t>1:5G-M80,1:5G-M81,1:5G-M82</t>
         </is>
       </c>
     </row>
@@ -17631,7 +17631,7 @@
       </c>
       <c r="F647" t="inlineStr">
         <is>
-          <t>1:M80,1:M81,1:M82</t>
+          <t>1:5G-M80,1:5G-M81,1:5G-M82</t>
         </is>
       </c>
     </row>
@@ -17675,7 +17675,7 @@
       </c>
       <c r="F649" t="inlineStr">
         <is>
-          <t>1:M80,1:M81,1:M82</t>
+          <t>1:5G-M80,1:5G-M81,1:5G-M82</t>
         </is>
       </c>
     </row>
@@ -17719,7 +17719,7 @@
       </c>
       <c r="F651" t="inlineStr">
         <is>
-          <t>1:M80,1:M81,1:M82</t>
+          <t>1:5G-M80,1:5G-M81,1:5G-M82</t>
         </is>
       </c>
     </row>
@@ -17763,7 +17763,7 @@
       </c>
       <c r="F653" t="inlineStr">
         <is>
-          <t>1:M80,1:M81,1:M82</t>
+          <t>1:5G-M80,1:5G-M81,1:5G-M82</t>
         </is>
       </c>
     </row>
@@ -17810,7 +17810,7 @@
       </c>
       <c r="F655" t="inlineStr">
         <is>
-          <t>1:M80,1:M81,1:M82</t>
+          <t>1:5G-M80,1:5G-M81,1:5G-M82</t>
         </is>
       </c>
     </row>
@@ -17857,7 +17857,7 @@
       </c>
       <c r="F657" t="inlineStr">
         <is>
-          <t>1:M80,1:M81,1:M82</t>
+          <t>1:5G-M80,1:5G-M81,1:5G-M82</t>
         </is>
       </c>
     </row>
@@ -17901,7 +17901,7 @@
       </c>
       <c r="F659" t="inlineStr">
         <is>
-          <t>1:M80,1:M81,1:M82</t>
+          <t>1:5G-M80,1:5G-M81,1:5G-M82</t>
         </is>
       </c>
     </row>
@@ -17945,7 +17945,7 @@
       </c>
       <c r="F661" t="inlineStr">
         <is>
-          <t>1:M80,1:M81,1:M82</t>
+          <t>1:5G-M80,1:5G-M81,1:5G-M82</t>
         </is>
       </c>
     </row>
@@ -17989,7 +17989,7 @@
       </c>
       <c r="F663" t="inlineStr">
         <is>
-          <t>1:M80,1:M81,1:M82</t>
+          <t>1:5G-M80,1:5G-M81,1:5G-M82</t>
         </is>
       </c>
     </row>
@@ -18033,7 +18033,7 @@
       </c>
       <c r="F665" t="inlineStr">
         <is>
-          <t>1:M80,1:M81,1:M82</t>
+          <t>1:5G-M80,1:5G-M81,1:5G-M82</t>
         </is>
       </c>
     </row>
@@ -18077,7 +18077,7 @@
       </c>
       <c r="F667" t="inlineStr">
         <is>
-          <t>1:M80,1:M81,1:M82</t>
+          <t>1:5G-M80,1:5G-M81,1:5G-M82</t>
         </is>
       </c>
     </row>
@@ -18121,7 +18121,7 @@
       </c>
       <c r="F669" t="inlineStr">
         <is>
-          <t>1:M80,1:M81,1:M82</t>
+          <t>1:5G-M80,1:5G-M81,1:5G-M82</t>
         </is>
       </c>
     </row>
@@ -18167,7 +18167,7 @@
       </c>
       <c r="F671" t="inlineStr">
         <is>
-          <t>1:M80,1:M81,1:M82</t>
+          <t>1:5G-M80,1:5G-M81,1:5G-M82</t>
         </is>
       </c>
     </row>
@@ -18235,7 +18235,7 @@
       </c>
       <c r="F674" t="inlineStr">
         <is>
-          <t>1:M83,1:M84,1:M85,1:M86</t>
+          <t>1:5G-M83,1:5G-M84,1:5G-M85,1:5G-M86</t>
         </is>
       </c>
     </row>
@@ -18279,7 +18279,7 @@
       </c>
       <c r="F676" t="inlineStr">
         <is>
-          <t>1:M83,1:M84,1:M85,1:M86</t>
+          <t>1:5G-M83,1:5G-M84,1:5G-M85,1:5G-M86</t>
         </is>
       </c>
     </row>
@@ -18323,7 +18323,7 @@
       </c>
       <c r="F678" t="inlineStr">
         <is>
-          <t>1:M83,1:M84,1:M85,1:M86</t>
+          <t>1:5G-M83,1:5G-M84,1:5G-M85,1:5G-M86</t>
         </is>
       </c>
     </row>
@@ -18390,7 +18390,7 @@
       </c>
       <c r="F681" t="inlineStr">
         <is>
-          <t>1:M87,1:M88,1:M89</t>
+          <t>1:5G-M87,1:5G-M88,1:5G-M89</t>
         </is>
       </c>
     </row>
@@ -18434,7 +18434,7 @@
       </c>
       <c r="F683" t="inlineStr">
         <is>
-          <t>1:M87,1:M88,1:M89</t>
+          <t>1:5G-M87,1:5G-M88,1:5G-M89</t>
         </is>
       </c>
     </row>
@@ -18478,7 +18478,7 @@
       </c>
       <c r="F685" t="inlineStr">
         <is>
-          <t>1:M87,1:M88,1:M89</t>
+          <t>1:5G-M87,1:5G-M88,1:5G-M89</t>
         </is>
       </c>
     </row>
@@ -18522,7 +18522,7 @@
       </c>
       <c r="F687" t="inlineStr">
         <is>
-          <t>1:M87,1:M88,1:M89</t>
+          <t>1:5G-M87,1:5G-M88,1:5G-M89</t>
         </is>
       </c>
     </row>
@@ -18567,7 +18567,7 @@
       </c>
       <c r="F689" t="inlineStr">
         <is>
-          <t>1:M87,1:M88,1:M89</t>
+          <t>1:5G-M87,1:5G-M88,1:5G-M89</t>
         </is>
       </c>
     </row>
@@ -18611,7 +18611,7 @@
       </c>
       <c r="F691" t="inlineStr">
         <is>
-          <t>1:M87,1:M88,1:M89</t>
+          <t>1:5G-M87,1:5G-M88,1:5G-M89</t>
         </is>
       </c>
     </row>
@@ -18655,7 +18655,7 @@
       </c>
       <c r="F693" t="inlineStr">
         <is>
-          <t>1:M87,1:M88,1:M89</t>
+          <t>1:5G-M87,1:5G-M88,1:5G-M89</t>
         </is>
       </c>
     </row>
@@ -18699,7 +18699,7 @@
       </c>
       <c r="F695" t="inlineStr">
         <is>
-          <t>1:M87,1:M88,1:M89</t>
+          <t>1:5G-M87,1:5G-M88,1:5G-M89</t>
         </is>
       </c>
     </row>
@@ -18743,7 +18743,7 @@
       </c>
       <c r="F697" t="inlineStr">
         <is>
-          <t>1:M87,1:M88,1:M89</t>
+          <t>1:5G-M87,1:5G-M88,1:5G-M89</t>
         </is>
       </c>
     </row>
@@ -18787,7 +18787,7 @@
       </c>
       <c r="F699" t="inlineStr">
         <is>
-          <t>1:M87,1:M88,1:M89</t>
+          <t>1:5G-M87,1:5G-M88,1:5G-M89</t>
         </is>
       </c>
     </row>
@@ -18831,7 +18831,7 @@
       </c>
       <c r="F701" t="inlineStr">
         <is>
-          <t>1:M87,1:M88,1:M89</t>
+          <t>1:5G-M87,1:5G-M88,1:5G-M89</t>
         </is>
       </c>
     </row>
@@ -18875,7 +18875,7 @@
       </c>
       <c r="F703" t="inlineStr">
         <is>
-          <t>1:M87,1:M88,1:M89</t>
+          <t>1:5G-M87,1:5G-M88,1:5G-M89</t>
         </is>
       </c>
     </row>
@@ -18920,7 +18920,7 @@
       </c>
       <c r="F705" t="inlineStr">
         <is>
-          <t>1:M87,1:M88,1:M89</t>
+          <t>1:5G-M87,1:5G-M88,1:5G-M89</t>
         </is>
       </c>
     </row>
@@ -18966,7 +18966,7 @@
       </c>
       <c r="F707" t="inlineStr">
         <is>
-          <t>1:M87,1:M88,1:M89</t>
+          <t>1:5G-M87,1:5G-M88,1:5G-M89</t>
         </is>
       </c>
     </row>
@@ -19057,7 +19057,7 @@
       </c>
       <c r="F711" t="inlineStr">
         <is>
-          <t>1:M90,1:M91,1:M92,1:M93,1:M94</t>
+          <t>1:5G-M90,1:5G-M91,1:5G-M92,1:5G-M93,1:5G-M94</t>
         </is>
       </c>
     </row>
@@ -19101,7 +19101,7 @@
       </c>
       <c r="F713" t="inlineStr">
         <is>
-          <t>1:M90,1:M91,1:M92,1:M93,1:M94</t>
+          <t>1:5G-M90,1:5G-M91,1:5G-M92,1:5G-M93,1:5G-M94</t>
         </is>
       </c>
     </row>
@@ -19167,7 +19167,7 @@
       </c>
       <c r="F716" t="inlineStr">
         <is>
-          <t>1:M95,1:M96,1:M97,1:M98,1:M99</t>
+          <t>1:5G-M95,1:5G-M96,1:5G-M97,1:5G-M98,1:5G-M99</t>
         </is>
       </c>
     </row>
@@ -19211,7 +19211,7 @@
       </c>
       <c r="F718" t="inlineStr">
         <is>
-          <t>1:M95,1:M96,1:M97,1:M98,1:M99</t>
+          <t>1:5G-M95,1:5G-M96,1:5G-M97,1:5G-M98,1:5G-M99</t>
         </is>
       </c>
     </row>
@@ -19255,7 +19255,7 @@
       </c>
       <c r="F720" t="inlineStr">
         <is>
-          <t>1:M95,1:M96,1:M97,1:M98,1:M99</t>
+          <t>1:5G-M95,1:5G-M96,1:5G-M97,1:5G-M98,1:5G-M99</t>
         </is>
       </c>
     </row>
@@ -19299,7 +19299,7 @@
       </c>
       <c r="F722" t="inlineStr">
         <is>
-          <t>1:M95,1:M96,1:M97,1:M98,1:M99</t>
+          <t>1:5G-M95,1:5G-M96,1:5G-M97,1:5G-M98,1:5G-M99</t>
         </is>
       </c>
     </row>
@@ -19343,7 +19343,7 @@
       </c>
       <c r="F724" t="inlineStr">
         <is>
-          <t>1:M95,1:M96,1:M97,1:M98,1:M99</t>
+          <t>1:5G-M95,1:5G-M96,1:5G-M97,1:5G-M98,1:5G-M99</t>
         </is>
       </c>
     </row>
@@ -19387,7 +19387,7 @@
       </c>
       <c r="F726" t="inlineStr">
         <is>
-          <t>1:M95,1:M96,1:M97,1:M98,1:M99</t>
+          <t>1:5G-M95,1:5G-M96,1:5G-M97,1:5G-M98,1:5G-M99</t>
         </is>
       </c>
     </row>
@@ -19475,7 +19475,7 @@
       </c>
       <c r="F730" t="inlineStr">
         <is>
-          <t>1:M104,1:M105,1:M106,1:M107,1:M108,1:M109</t>
+          <t>1:5G-M104,1:5G-M105,1:5G-M106,1:5G-M107,1:5G-M108,1:5G-M109</t>
         </is>
       </c>
     </row>
@@ -19519,7 +19519,7 @@
       </c>
       <c r="F732" t="inlineStr">
         <is>
-          <t>1:M104,1:M105,1:M106,1:M107,1:M108,1:M109</t>
+          <t>1:5G-M104,1:5G-M105,1:5G-M106,1:5G-M107,1:5G-M108,1:5G-M109</t>
         </is>
       </c>
     </row>
@@ -19563,7 +19563,7 @@
       </c>
       <c r="F734" t="inlineStr">
         <is>
-          <t>1:M104,1:M105,1:M106,1:M107,1:M108,1:M109</t>
+          <t>1:5G-M104,1:5G-M105,1:5G-M106,1:5G-M107,1:5G-M108,1:5G-M109</t>
         </is>
       </c>
     </row>
@@ -19607,7 +19607,7 @@
       </c>
       <c r="F736" t="inlineStr">
         <is>
-          <t>1:M104,1:M105,1:M106,1:M107,1:M108,1:M109</t>
+          <t>1:5G-M104,1:5G-M105,1:5G-M106,1:5G-M107,1:5G-M108,1:5G-M109</t>
         </is>
       </c>
     </row>
@@ -19651,7 +19651,7 @@
       </c>
       <c r="F738" t="inlineStr">
         <is>
-          <t>1:M104,1:M105,1:M106,1:M107,1:M108,1:M109</t>
+          <t>1:5G-M104,1:5G-M105,1:5G-M106,1:5G-M107,1:5G-M108,1:5G-M109</t>
         </is>
       </c>
     </row>
@@ -19695,7 +19695,7 @@
       </c>
       <c r="F740" t="inlineStr">
         <is>
-          <t>1:M104,1:M105,1:M106,1:M107,1:M108,1:M109</t>
+          <t>1:5G-M104,1:5G-M105,1:5G-M106,1:5G-M107,1:5G-M108,1:5G-M109</t>
         </is>
       </c>
     </row>
@@ -19739,7 +19739,7 @@
       </c>
       <c r="F742" t="inlineStr">
         <is>
-          <t>1:M104,1:M105,1:M106,1:M107,1:M108,1:M109</t>
+          <t>1:5G-M104,1:5G-M105,1:5G-M106,1:5G-M107,1:5G-M108,1:5G-M109</t>
         </is>
       </c>
     </row>
@@ -19783,7 +19783,7 @@
       </c>
       <c r="F744" t="inlineStr">
         <is>
-          <t>1:M104,1:M105,1:M106,1:M107,1:M108,1:M109</t>
+          <t>1:5G-M104,1:5G-M105,1:5G-M106,1:5G-M107,1:5G-M108,1:5G-M109</t>
         </is>
       </c>
     </row>
@@ -19827,7 +19827,7 @@
       </c>
       <c r="F746" t="inlineStr">
         <is>
-          <t>1:M104,1:M105,1:M106,1:M107,1:M108,1:M109</t>
+          <t>1:5G-M104,1:5G-M105,1:5G-M106,1:5G-M107,1:5G-M108,1:5G-M109</t>
         </is>
       </c>
     </row>
@@ -19871,7 +19871,7 @@
       </c>
       <c r="F748" t="inlineStr">
         <is>
-          <t>1:M104,1:M105,1:M106,1:M107,1:M108,1:M109</t>
+          <t>1:5G-M104,1:5G-M105,1:5G-M106,1:5G-M107,1:5G-M108,1:5G-M109</t>
         </is>
       </c>
     </row>
@@ -19915,7 +19915,7 @@
       </c>
       <c r="F750" t="inlineStr">
         <is>
-          <t>1:M104,1:M105,1:M106,1:M107,1:M108,1:M109</t>
+          <t>1:5G-M104,1:5G-M105,1:5G-M106,1:5G-M107,1:5G-M108,1:5G-M109</t>
         </is>
       </c>
     </row>
@@ -19959,7 +19959,7 @@
       </c>
       <c r="F752" t="inlineStr">
         <is>
-          <t>1:M104,1:M105,1:M106,1:M107,1:M108,1:M109</t>
+          <t>1:5G-M104,1:5G-M105,1:5G-M106,1:5G-M107,1:5G-M108,1:5G-M109</t>
         </is>
       </c>
     </row>
@@ -20003,7 +20003,7 @@
       </c>
       <c r="F754" t="inlineStr">
         <is>
-          <t>1:M104,1:M105,1:M106,1:M107,1:M108,1:M109</t>
+          <t>1:5G-M104,1:5G-M105,1:5G-M106,1:5G-M107,1:5G-M108,1:5G-M109</t>
         </is>
       </c>
     </row>
@@ -20047,7 +20047,7 @@
       </c>
       <c r="F756" t="inlineStr">
         <is>
-          <t>1:M104,1:M105,1:M106,1:M107,1:M108,1:M109</t>
+          <t>1:5G-M104,1:5G-M105,1:5G-M106,1:5G-M107,1:5G-M108,1:5G-M109</t>
         </is>
       </c>
     </row>
@@ -20091,7 +20091,7 @@
       </c>
       <c r="F758" t="inlineStr">
         <is>
-          <t>1:M104,1:M105,1:M106,1:M107,1:M108,1:M109</t>
+          <t>1:5G-M104,1:5G-M105,1:5G-M106,1:5G-M107,1:5G-M108,1:5G-M109</t>
         </is>
       </c>
     </row>
@@ -20179,7 +20179,7 @@
       </c>
       <c r="F762" t="inlineStr">
         <is>
-          <t>1:M115,1:M116,1:M117,1:M118,1:M119,1:M120</t>
+          <t>1:5G-M115,1:5G-M116,1:5G-M117,1:5G-M118,1:5G-M119,1:5G-M120</t>
         </is>
       </c>
     </row>
@@ -20223,7 +20223,7 @@
       </c>
       <c r="F764" t="inlineStr">
         <is>
-          <t>1:M115,1:M116,1:M117,1:M118,1:M119,1:M120</t>
+          <t>1:5G-M115,1:5G-M116,1:5G-M117,1:5G-M118,1:5G-M119,1:5G-M120</t>
         </is>
       </c>
     </row>
@@ -20267,7 +20267,7 @@
       </c>
       <c r="F766" t="inlineStr">
         <is>
-          <t>1:M115,1:M116,1:M117,1:M118,1:M119,1:M120</t>
+          <t>1:5G-M115,1:5G-M116,1:5G-M117,1:5G-M118,1:5G-M119,1:5G-M120</t>
         </is>
       </c>
     </row>
@@ -20311,7 +20311,7 @@
       </c>
       <c r="F768" t="inlineStr">
         <is>
-          <t>1:M115,1:M116,1:M117,1:M118,1:M119,1:M120</t>
+          <t>1:5G-M115,1:5G-M116,1:5G-M117,1:5G-M118,1:5G-M119,1:5G-M120</t>
         </is>
       </c>
     </row>
@@ -20355,7 +20355,7 @@
       </c>
       <c r="F770" t="inlineStr">
         <is>
-          <t>1:M115,1:M116,1:M117,1:M118,1:M119,1:M120</t>
+          <t>1:5G-M115,1:5G-M116,1:5G-M117,1:5G-M118,1:5G-M119,1:5G-M120</t>
         </is>
       </c>
     </row>
@@ -20399,7 +20399,7 @@
       </c>
       <c r="F772" t="inlineStr">
         <is>
-          <t>1:M115,1:M116,1:M117,1:M118,1:M119,1:M120</t>
+          <t>1:5G-M115,1:5G-M116,1:5G-M117,1:5G-M118,1:5G-M119,1:5G-M120</t>
         </is>
       </c>
     </row>
@@ -20443,7 +20443,7 @@
       </c>
       <c r="F774" t="inlineStr">
         <is>
-          <t>1:M115,1:M116,1:M117,1:M118,1:M119,1:M120</t>
+          <t>1:5G-M115,1:5G-M116,1:5G-M117,1:5G-M118,1:5G-M119,1:5G-M120</t>
         </is>
       </c>
     </row>
@@ -20487,7 +20487,7 @@
       </c>
       <c r="F776" t="inlineStr">
         <is>
-          <t>1:M115,1:M116,1:M117,1:M118,1:M119,1:M120</t>
+          <t>1:5G-M115,1:5G-M116,1:5G-M117,1:5G-M118,1:5G-M119,1:5G-M120</t>
         </is>
       </c>
     </row>
@@ -20531,7 +20531,7 @@
       </c>
       <c r="F778" t="inlineStr">
         <is>
-          <t>1:M115,1:M116,1:M117,1:M118,1:M119,1:M120</t>
+          <t>1:5G-M115,1:5G-M116,1:5G-M117,1:5G-M118,1:5G-M119,1:5G-M120</t>
         </is>
       </c>
     </row>
@@ -20575,7 +20575,7 @@
       </c>
       <c r="F780" t="inlineStr">
         <is>
-          <t>1:M115,1:M116,1:M117,1:M118,1:M119,1:M120</t>
+          <t>1:5G-M115,1:5G-M116,1:5G-M117,1:5G-M118,1:5G-M119,1:5G-M120</t>
         </is>
       </c>
     </row>
@@ -20619,7 +20619,7 @@
       </c>
       <c r="F782" t="inlineStr">
         <is>
-          <t>1:M115,1:M116,1:M117,1:M118,1:M119,1:M120</t>
+          <t>1:5G-M115,1:5G-M116,1:5G-M117,1:5G-M118,1:5G-M119,1:5G-M120</t>
         </is>
       </c>
     </row>
@@ -20664,7 +20664,7 @@
       </c>
       <c r="F784" t="inlineStr">
         <is>
-          <t>1:M115,1:M116,1:M117,1:M118,1:M119,1:M120</t>
+          <t>1:5G-M115,1:5G-M116,1:5G-M117,1:5G-M118,1:5G-M119,1:5G-M120</t>
         </is>
       </c>
     </row>
@@ -20714,7 +20714,7 @@
       </c>
       <c r="F786" t="inlineStr">
         <is>
-          <t>1:M115,1:M116,1:M117,1:M118,1:M119,1:M120</t>
+          <t>1:5G-M115,1:5G-M116,1:5G-M117,1:5G-M118,1:5G-M119,1:5G-M120</t>
         </is>
       </c>
     </row>
@@ -20762,7 +20762,7 @@
       </c>
       <c r="F788" t="inlineStr">
         <is>
-          <t>1:M115,1:M116,1:M117,1:M118,1:M119,1:M120</t>
+          <t>1:5G-M115,1:5G-M116,1:5G-M117,1:5G-M118,1:5G-M119,1:5G-M120</t>
         </is>
       </c>
     </row>
@@ -20810,7 +20810,7 @@
       </c>
       <c r="F790" t="inlineStr">
         <is>
-          <t>1:M115,1:M116,1:M117,1:M118,1:M119,1:M120</t>
+          <t>1:5G-M115,1:5G-M116,1:5G-M117,1:5G-M118,1:5G-M119,1:5G-M120</t>
         </is>
       </c>
     </row>
@@ -20857,7 +20857,7 @@
       </c>
       <c r="F792" t="inlineStr">
         <is>
-          <t>1:M115,1:M116,1:M117,1:M118,1:M119,1:M120</t>
+          <t>1:5G-M115,1:5G-M116,1:5G-M117,1:5G-M118,1:5G-M119,1:5G-M120</t>
         </is>
       </c>
     </row>
@@ -20901,7 +20901,7 @@
       </c>
       <c r="F794" t="inlineStr">
         <is>
-          <t>1:M115,1:M116,1:M117,1:M118,1:M119,1:M120</t>
+          <t>1:5G-M115,1:5G-M116,1:5G-M117,1:5G-M118,1:5G-M119,1:5G-M120</t>
         </is>
       </c>
     </row>
@@ -20945,7 +20945,7 @@
       </c>
       <c r="F796" t="inlineStr">
         <is>
-          <t>1:M115,1:M116,1:M117,1:M118,1:M119,1:M120</t>
+          <t>1:5G-M115,1:5G-M116,1:5G-M117,1:5G-M118,1:5G-M119,1:5G-M120</t>
         </is>
       </c>
     </row>
@@ -20989,7 +20989,7 @@
       </c>
       <c r="F798" t="inlineStr">
         <is>
-          <t>1:M115,1:M116,1:M117,1:M118,1:M119,1:M120</t>
+          <t>1:5G-M115,1:5G-M116,1:5G-M117,1:5G-M118,1:5G-M119,1:5G-M120</t>
         </is>
       </c>
     </row>
@@ -21035,7 +21035,7 @@
       </c>
       <c r="F800" t="inlineStr">
         <is>
-          <t>1:M115,1:M116,1:M117,1:M118,1:M119,1:M120</t>
+          <t>1:5G-M115,1:5G-M116,1:5G-M117,1:5G-M118,1:5G-M119,1:5G-M120</t>
         </is>
       </c>
     </row>
@@ -21082,7 +21082,7 @@
       </c>
       <c r="F802" t="inlineStr">
         <is>
-          <t>1:M115,1:M116,1:M117,1:M118,1:M119,1:M120</t>
+          <t>1:5G-M115,1:5G-M116,1:5G-M117,1:5G-M118,1:5G-M119,1:5G-M120</t>
         </is>
       </c>
     </row>
@@ -21126,7 +21126,7 @@
       </c>
       <c r="F804" t="inlineStr">
         <is>
-          <t>1:M115,1:M116,1:M117,1:M118,1:M119,1:M120</t>
+          <t>1:5G-M115,1:5G-M116,1:5G-M117,1:5G-M118,1:5G-M119,1:5G-M120</t>
         </is>
       </c>
     </row>
@@ -21192,7 +21192,7 @@
       </c>
       <c r="F807" t="inlineStr">
         <is>
-          <t>1:M121,1:M122,1:M123,1:M124,1:M125</t>
+          <t>1:5G-M121,1:5G-M122,1:5G-M123,1:5G-M124,1:5G-M125</t>
         </is>
       </c>
     </row>
@@ -21238,7 +21238,7 @@
       </c>
       <c r="F809" t="inlineStr">
         <is>
-          <t>1:M121,1:M122,1:M123,1:M124,1:M125</t>
+          <t>1:5G-M121,1:5G-M122,1:5G-M123,1:5G-M124,1:5G-M125</t>
         </is>
       </c>
     </row>
@@ -21304,7 +21304,7 @@
       </c>
       <c r="F812" t="inlineStr">
         <is>
-          <t>1:M126,1:M127,1:M128,1:M129</t>
+          <t>1:5G-M126,1:5G-M127,1:5G-M128,1:5G-M129</t>
         </is>
       </c>
     </row>
@@ -21351,7 +21351,7 @@
       </c>
       <c r="F814" t="inlineStr">
         <is>
-          <t>1:M126,1:M127,1:M128,1:M129</t>
+          <t>1:5G-M126,1:5G-M127,1:5G-M128,1:5G-M129</t>
         </is>
       </c>
     </row>
@@ -21417,7 +21417,7 @@
       </c>
       <c r="F817" t="inlineStr">
         <is>
-          <t>1:M134,1:M135,1:M136,1:M137</t>
+          <t>1:5G-M134,1:5G-M135,1:5G-M136,1:5G-M137</t>
         </is>
       </c>
     </row>
@@ -21461,7 +21461,7 @@
       </c>
       <c r="F819" t="inlineStr">
         <is>
-          <t>1:M134,1:M135,1:M136,1:M137</t>
+          <t>1:5G-M134,1:5G-M135,1:5G-M136,1:5G-M137</t>
         </is>
       </c>
     </row>
@@ -21505,7 +21505,7 @@
       </c>
       <c r="F821" t="inlineStr">
         <is>
-          <t>1:M134,1:M135,1:M136,1:M137</t>
+          <t>1:5G-M134,1:5G-M135,1:5G-M136,1:5G-M137</t>
         </is>
       </c>
     </row>
@@ -21593,7 +21593,7 @@
       </c>
       <c r="F825" t="inlineStr">
         <is>
-          <t>1:M142,1:M143,1:M144</t>
+          <t>1:5G-M142,1:5G-M143,1:5G-M144</t>
         </is>
       </c>
     </row>
@@ -21637,7 +21637,7 @@
       </c>
       <c r="F827" t="inlineStr">
         <is>
-          <t>1:M142,1:M143,1:M144</t>
+          <t>1:5G-M142,1:5G-M143,1:5G-M144</t>
         </is>
       </c>
     </row>
@@ -21681,7 +21681,7 @@
       </c>
       <c r="F829" t="inlineStr">
         <is>
-          <t>1:M142,1:M143,1:M144</t>
+          <t>1:5G-M142,1:5G-M143,1:5G-M144</t>
         </is>
       </c>
     </row>

</xml_diff>